<commit_message>
Guru99 demo page login changes completed.Add new customer WIP
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="NewCust" sheetId="2" r:id="rId2"/>
+    <sheet name="EditCust" sheetId="3" r:id="rId3"/>
+    <sheet name="DeleteCust" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
   <si>
     <t>testcaseID</t>
   </si>
@@ -75,10 +78,346 @@
     <t>message</t>
   </si>
   <si>
-    <t>Logged in successfully</t>
-  </si>
-  <si>
-    <t>Invalid user or password</t>
+    <t>User or Password is not valid</t>
+  </si>
+  <si>
+    <t>Pass - User or Password is not valid</t>
+  </si>
+  <si>
+    <t>Guru99 Bank Manager HomePage</t>
+  </si>
+  <si>
+    <t>Blank user</t>
+  </si>
+  <si>
+    <t>Blank password</t>
+  </si>
+  <si>
+    <t>Blank user credential</t>
+  </si>
+  <si>
+    <t>NytyygfF</t>
+  </si>
+  <si>
+    <t>mngr564377</t>
+  </si>
+  <si>
+    <t>Pass - Guru99 Bank Manager HomePage</t>
+  </si>
+  <si>
+    <t>User-ID must not be blank</t>
+  </si>
+  <si>
+    <t>Password must not be blank</t>
+  </si>
+  <si>
+    <t>User-ID must not be blankPassword must not be blank</t>
+  </si>
+  <si>
+    <t>Pass - User-ID must not be blank</t>
+  </si>
+  <si>
+    <t>Pass - Password must not be blank</t>
+  </si>
+  <si>
+    <t>Pass - User-ID must not be blankPassword must not be blank</t>
+  </si>
+  <si>
+    <t>custName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>mobNo</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>custid</t>
+  </si>
+  <si>
+    <t>Valid customer creation</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Keith</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>19 5th main KT layout</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>87 9th cross TM road</t>
+  </si>
+  <si>
+    <t>Mysore</t>
+  </si>
+  <si>
+    <t>jim@test.com</t>
+  </si>
+  <si>
+    <t>54 7th main DR road</t>
+  </si>
+  <si>
+    <t>Mangalore</t>
+  </si>
+  <si>
+    <t>keith@test.com</t>
+  </si>
+  <si>
+    <t>Blank customer name</t>
+  </si>
+  <si>
+    <t>Numbers in customer name</t>
+  </si>
+  <si>
+    <t>Special characters in customer name</t>
+  </si>
+  <si>
+    <t>Customer name exceeding 25 characters</t>
+  </si>
+  <si>
+    <t>Blank gender</t>
+  </si>
+  <si>
+    <t>Blank DOB</t>
+  </si>
+  <si>
+    <t>Future DOB</t>
+  </si>
+  <si>
+    <t>Blank address</t>
+  </si>
+  <si>
+    <t>Numbers in address</t>
+  </si>
+  <si>
+    <t>Special characters in address</t>
+  </si>
+  <si>
+    <t>Address exceeding 50 characters</t>
+  </si>
+  <si>
+    <t>Blank city</t>
+  </si>
+  <si>
+    <t>Numbers in city</t>
+  </si>
+  <si>
+    <t>Special characters in city</t>
+  </si>
+  <si>
+    <t>City exceeding 25 characters</t>
+  </si>
+  <si>
+    <t>Numbers in state</t>
+  </si>
+  <si>
+    <t>Blank state</t>
+  </si>
+  <si>
+    <t>Special characters in state</t>
+  </si>
+  <si>
+    <t>State exceeding 25 characters</t>
+  </si>
+  <si>
+    <t>Blank pin</t>
+  </si>
+  <si>
+    <t>Characters in pin</t>
+  </si>
+  <si>
+    <t>Special characters in pin</t>
+  </si>
+  <si>
+    <t>Pin exceeding 6 digits</t>
+  </si>
+  <si>
+    <t>Pin less than 6 digits</t>
+  </si>
+  <si>
+    <t>Blank mobile number</t>
+  </si>
+  <si>
+    <t>Characters in mobile number</t>
+  </si>
+  <si>
+    <t>Special characters in mobile number</t>
+  </si>
+  <si>
+    <t>Mobile number exc eeding 15 digits</t>
+  </si>
+  <si>
+    <t>Mobile number less than 5 digits</t>
+  </si>
+  <si>
+    <t>Blank email id</t>
+  </si>
+  <si>
+    <t>Invalid email id with out @</t>
+  </si>
+  <si>
+    <t>Invalid email id without domain name</t>
+  </si>
+  <si>
+    <t>Invalid email id</t>
+  </si>
+  <si>
+    <t>Only spaces in customer name</t>
+  </si>
+  <si>
+    <t>Only spaces in address</t>
+  </si>
+  <si>
+    <t>Only spaces in city</t>
+  </si>
+  <si>
+    <t>Only spaces in state</t>
+  </si>
+  <si>
+    <t>Only spaces in pin</t>
+  </si>
+  <si>
+    <t>Only spaces in mobile number</t>
+  </si>
+  <si>
+    <t>Only spaces in email id</t>
+  </si>
+  <si>
+    <t>Only spaces in password</t>
+  </si>
+  <si>
+    <t>Email id exceeding 10 characters</t>
+  </si>
+  <si>
+    <t>Password exceeding 10 characters</t>
+  </si>
+  <si>
+    <t>Password with numbers,characters and special characters</t>
+  </si>
+  <si>
+    <t>All fields blank</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>ji@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t>10 GJ road</t>
+  </si>
+  <si>
+    <t>98 WD layout</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>67 LN road</t>
+  </si>
+  <si>
+    <t>$&amp;^*(</t>
+  </si>
+  <si>
+    <t>90 MB road</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>SaaaaaaannnnnnnnvvvvviiiiS</t>
+  </si>
+  <si>
+    <t>75 8th main KJ road</t>
+  </si>
+  <si>
+    <t>sanvi@test.com</t>
+  </si>
+  <si>
+    <t>Mohan</t>
+  </si>
+  <si>
+    <t>65 19t main TR layout</t>
+  </si>
+  <si>
+    <t>Mandya</t>
+  </si>
+  <si>
+    <t>mohan@test.com</t>
+  </si>
+  <si>
+    <t>Drona</t>
+  </si>
+  <si>
+    <t>78 NCD layout</t>
+  </si>
+  <si>
+    <t>Bijapur</t>
+  </si>
+  <si>
+    <t>drona@test.com</t>
+  </si>
+  <si>
+    <t>Keya</t>
+  </si>
+  <si>
+    <t>98 6th main DVG road</t>
+  </si>
+  <si>
+    <t>keya@test.com</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Customer Created successfully!</t>
+  </si>
+  <si>
+    <t>Joshna</t>
+  </si>
+  <si>
+    <t>josh@test.com</t>
   </si>
 </sst>
 </file>
@@ -102,7 +441,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,8 +454,43 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -139,16 +513,130 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -430,18 +918,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="51.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -484,9 +973,11 @@
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -505,9 +996,11 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -526,9 +1019,11 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -547,15 +1042,1434 @@
         <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3:C5" r:id="rId2" display="http://demo.guru99.com/v4/"/>
+    <hyperlink ref="C6:C8" r:id="rId3" display="http://demo.guru99.com/v4/"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="11">
+        <v>29969</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="1">
+        <v>566721</v>
+      </c>
+      <c r="J2" s="1">
+        <v>7771232345</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="11">
+        <v>30715</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="1">
+        <v>789067</v>
+      </c>
+      <c r="J3" s="1">
+        <v>7778907689</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="11">
+        <v>28921</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="1">
+        <v>890789</v>
+      </c>
+      <c r="J4" s="1">
+        <v>7771237890</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="11">
+        <v>31855</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="1">
+        <v>237876</v>
+      </c>
+      <c r="J5" s="1">
+        <v>9991237890</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="11">
+        <v>31481</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="1">
+        <v>667897</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5556789087</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="1">
+        <v>12334</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="11">
+        <v>30477</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="1">
+        <v>788767</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5554567897</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="11">
+        <v>28690</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="1">
+        <v>897654</v>
+      </c>
+      <c r="J8" s="1">
+        <v>4448960786</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="11">
+        <v>29938</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="1">
+        <v>765897</v>
+      </c>
+      <c r="J9" s="1">
+        <v>4447895432</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="11">
+        <v>32527</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="1">
+        <v>789123</v>
+      </c>
+      <c r="J10" s="1">
+        <v>7779081234</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="1">
+        <v>678234</v>
+      </c>
+      <c r="J11" s="1">
+        <v>7776892313</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="11">
+        <v>235197</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="1">
+        <v>786889</v>
+      </c>
+      <c r="J12" s="1">
+        <v>7771236789</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K4" r:id="rId3"/>
+    <hyperlink ref="K5" r:id="rId4"/>
+    <hyperlink ref="K6" r:id="rId5"/>
+    <hyperlink ref="K7" r:id="rId6"/>
+    <hyperlink ref="K8" r:id="rId7"/>
+    <hyperlink ref="K9" r:id="rId8"/>
+    <hyperlink ref="K10" r:id="rId9"/>
+    <hyperlink ref="K11" r:id="rId10"/>
+    <hyperlink ref="K12" r:id="rId11"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New scenarios for add New Customer
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" r:id="rId1" sheetId="1"/>
-    <sheet name="NewCust" r:id="rId2" sheetId="2"/>
-    <sheet name="EditCust" r:id="rId3" sheetId="3"/>
-    <sheet name="DeleteCust" r:id="rId4" sheetId="4"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="NewCust" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="EditCust" sheetId="3" r:id="rId4"/>
+    <sheet name="DeleteCust" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NewCust!$H$1:$H$50</definedName>
+  </definedNames>
+  <calcPr calcId="171027"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="302">
   <si>
     <t>testcaseID</t>
   </si>
@@ -192,9 +197,6 @@
     <t>Mangalore</t>
   </si>
   <si>
-    <t>keith@test.com</t>
-  </si>
-  <si>
     <t>Blank customer name</t>
   </si>
   <si>
@@ -219,9 +221,6 @@
     <t>Blank address</t>
   </si>
   <si>
-    <t>Numbers in address</t>
-  </si>
-  <si>
     <t>Special characters in address</t>
   </si>
   <si>
@@ -384,9 +383,6 @@
     <t>Mandya</t>
   </si>
   <si>
-    <t>mohan@test.com</t>
-  </si>
-  <si>
     <t>Drona</t>
   </si>
   <si>
@@ -396,9 +392,6 @@
     <t>Bijapur</t>
   </si>
   <si>
-    <t>drona@test.com</t>
-  </si>
-  <si>
     <t>Keya</t>
   </si>
   <si>
@@ -411,20 +404,543 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Customer Created successfully!</t>
-  </si>
-  <si>
     <t>Joshna</t>
   </si>
   <si>
-    <t>josh@test.com</t>
+    <t>Customer Registered Successfully!!!</t>
+  </si>
+  <si>
+    <t>Customer name must not be blank</t>
+  </si>
+  <si>
+    <t>First character can not have space</t>
+  </si>
+  <si>
+    <t>Numbers are not allowed</t>
+  </si>
+  <si>
+    <t>Special characters are not allowed</t>
+  </si>
+  <si>
+    <t>Date Field must not be blank</t>
+  </si>
+  <si>
+    <t>Sujith</t>
+  </si>
+  <si>
+    <t>Kochi</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Address Field must not be blank</t>
+  </si>
+  <si>
+    <t>Only numbers in address</t>
+  </si>
+  <si>
+    <t>City Field must not be blank</t>
+  </si>
+  <si>
+    <t>State must not be blank</t>
+  </si>
+  <si>
+    <t>PIN Code must not be blank</t>
+  </si>
+  <si>
+    <t>Characters are not allowed</t>
+  </si>
+  <si>
+    <t>PIN Code must have 6 Digits</t>
+  </si>
+  <si>
+    <t>Mobile no must not be blank</t>
+  </si>
+  <si>
+    <t>Email-ID must not be blank</t>
+  </si>
+  <si>
+    <t>Email-ID is not valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer name must not be blankDate Field must not be blankAddress Field must not be blank
+City Field must not be blankState must not be blankPIN Code must not be blankMobile no must not be blankEmail-ID must not be blankPassword must not be blank
+</t>
+  </si>
+  <si>
+    <t>Om</t>
+  </si>
+  <si>
+    <t>656 8th main DU road</t>
+  </si>
+  <si>
+    <t>Spana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           </t>
+  </si>
+  <si>
+    <t>Cuttak</t>
+  </si>
+  <si>
+    <t>Orissa</t>
+  </si>
+  <si>
+    <t>Bala</t>
+  </si>
+  <si>
+    <t>Kolkata</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t>bala@test.com</t>
+  </si>
+  <si>
+    <t>Neelam</t>
+  </si>
+  <si>
+    <t>##%^$,</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Sonia</t>
+  </si>
+  <si>
+    <t>67 Green House 5A cross 7D main road Near HG towers Ambedakar nagar</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>Meher</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>Ketan</t>
+  </si>
+  <si>
+    <t>Vineet</t>
+  </si>
+  <si>
+    <t>Joy</t>
+  </si>
+  <si>
+    <t>Don</t>
+  </si>
+  <si>
+    <t>Chandan</t>
+  </si>
+  <si>
+    <t>Pari</t>
+  </si>
+  <si>
+    <t>Amar</t>
+  </si>
+  <si>
+    <t>Varun</t>
+  </si>
+  <si>
+    <t>Zaheer</t>
+  </si>
+  <si>
+    <t>Virat</t>
+  </si>
+  <si>
+    <t>Anu</t>
+  </si>
+  <si>
+    <t>Sanya</t>
+  </si>
+  <si>
+    <t>Pamela</t>
+  </si>
+  <si>
+    <t>Rekha</t>
+  </si>
+  <si>
+    <t>Kiara</t>
+  </si>
+  <si>
+    <t>Hansika</t>
+  </si>
+  <si>
+    <t>Kiran</t>
+  </si>
+  <si>
+    <t>Neha</t>
+  </si>
+  <si>
+    <t>Laila</t>
+  </si>
+  <si>
+    <t>Binny</t>
+  </si>
+  <si>
+    <t>Ronika</t>
+  </si>
+  <si>
+    <t>Roohi</t>
+  </si>
+  <si>
+    <t>Veeru</t>
+  </si>
+  <si>
+    <t>Darshan</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>Anoop</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Prerana</t>
+  </si>
+  <si>
+    <t>P@ssw0r3$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
+  <si>
+    <t>Password1234</t>
+  </si>
+  <si>
+    <t>vin@test.com</t>
+  </si>
+  <si>
+    <t>raj@test.com</t>
+  </si>
+  <si>
+    <t>ket@test.com</t>
+  </si>
+  <si>
+    <t>joy@test.com</t>
+  </si>
+  <si>
+    <t>don@test.com</t>
+  </si>
+  <si>
+    <t>cha@test.com</t>
+  </si>
+  <si>
+    <t>par@test.com</t>
+  </si>
+  <si>
+    <t>ama@test.com</t>
+  </si>
+  <si>
+    <t>var@test.com</t>
+  </si>
+  <si>
+    <t>zah@test.com</t>
+  </si>
+  <si>
+    <t>vir@test.com</t>
+  </si>
+  <si>
+    <t>anu@test.com</t>
+  </si>
+  <si>
+    <t>san@test.com</t>
+  </si>
+  <si>
+    <t>pam@test.com</t>
+  </si>
+  <si>
+    <t>rek@test.com</t>
+  </si>
+  <si>
+    <t>kia@test.com</t>
+  </si>
+  <si>
+    <t>han@test.com</t>
+  </si>
+  <si>
+    <t>kir@test.com</t>
+  </si>
+  <si>
+    <t>neh@test.com</t>
+  </si>
+  <si>
+    <t>lai@test.com</t>
+  </si>
+  <si>
+    <t>bin@test.com</t>
+  </si>
+  <si>
+    <t>ron@test.com</t>
+  </si>
+  <si>
+    <t>roo@test.com</t>
+  </si>
+  <si>
+    <t>vee@test.com</t>
+  </si>
+  <si>
+    <t>dar@test.com</t>
+  </si>
+  <si>
+    <t>ali@test.com</t>
+  </si>
+  <si>
+    <t>ano@test.com</t>
+  </si>
+  <si>
+    <t>tim@test.com</t>
+  </si>
+  <si>
+    <t>pre@test.com</t>
+  </si>
+  <si>
+    <t>jos@test.com</t>
+  </si>
+  <si>
+    <t>kei@test.com</t>
+  </si>
+  <si>
+    <t>moh@test.com</t>
+  </si>
+  <si>
+    <t>dro@test.com</t>
+  </si>
+  <si>
+    <t>suj@test.com</t>
+  </si>
+  <si>
+    <t>sap@test.com</t>
+  </si>
+  <si>
+    <t>nee@test.com</t>
+  </si>
+  <si>
+    <t>son@test.com</t>
+  </si>
+  <si>
+    <t>meh@test.com</t>
+  </si>
+  <si>
+    <t>34 8th main road KT road</t>
+  </si>
+  <si>
+    <t>Calicut</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Madurai</t>
+  </si>
+  <si>
+    <t>Salem</t>
+  </si>
+  <si>
+    <t>Nellore</t>
+  </si>
+  <si>
+    <t>Srinagar</t>
+  </si>
+  <si>
+    <t>Jammu Kashmir</t>
+  </si>
+  <si>
+    <t>Shimoga</t>
+  </si>
+  <si>
+    <t>Surat</t>
+  </si>
+  <si>
+    <t>Gujrat</t>
+  </si>
+  <si>
+    <t>Nagpur</t>
+  </si>
+  <si>
+    <t>Patna</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>Agra</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>Rajkot</t>
+  </si>
+  <si>
+    <t>Gaya</t>
+  </si>
+  <si>
+    <t>Tenali</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Gulbarga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t>$$*&amp;^%</t>
+  </si>
+  <si>
+    <t>MaduraiMaduraiIndiaTamilNadu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>%^%$*())</t>
+  </si>
+  <si>
+    <t>IndiaGujratgujgujgujgujIndia</t>
+  </si>
+  <si>
+    <t>om@test.com</t>
+  </si>
+  <si>
+    <t>#&amp;**&amp;^</t>
+  </si>
+  <si>
+    <t>rrte</t>
+  </si>
+  <si>
+    <t>54 9th cross VD road</t>
+  </si>
+  <si>
+    <t>87 6th main BNM layout</t>
+  </si>
+  <si>
+    <t>76 Kalyan nagar</t>
+  </si>
+  <si>
+    <t>76 HT road</t>
+  </si>
+  <si>
+    <t>54 VR road</t>
+  </si>
+  <si>
+    <t>89 7th cross ABN layout</t>
+  </si>
+  <si>
+    <t>898 8th main BT road</t>
+  </si>
+  <si>
+    <t>87 VC road</t>
+  </si>
+  <si>
+    <t>76 SD road</t>
+  </si>
+  <si>
+    <t>43 SH layout</t>
+  </si>
+  <si>
+    <t>98 5th main PT road</t>
+  </si>
+  <si>
+    <t>65 NCD layout</t>
+  </si>
+  <si>
+    <t>88 NC road</t>
+  </si>
+  <si>
+    <t>99 KDC layout</t>
+  </si>
+  <si>
+    <t>657 NT road</t>
+  </si>
+  <si>
+    <t>54 18t main KD road</t>
+  </si>
+  <si>
+    <t>56 PD road</t>
+  </si>
+  <si>
+    <t>77 TD road</t>
+  </si>
+  <si>
+    <t>789 SD road</t>
+  </si>
+  <si>
+    <t>23 RD road</t>
+  </si>
+  <si>
+    <t>776 DC road</t>
+  </si>
+  <si>
+    <t>82 10th main GD road</t>
+  </si>
+  <si>
+    <t>81 11th cross ND road</t>
+  </si>
+  <si>
+    <t>73 PD road</t>
+  </si>
+  <si>
+    <t>912 SC layout</t>
+  </si>
+  <si>
+    <t>32 AT road</t>
+  </si>
+  <si>
+    <t>88 VC road</t>
+  </si>
+  <si>
+    <t>55 MNB layout</t>
+  </si>
+  <si>
+    <t>45 PRT layout</t>
+  </si>
+  <si>
+    <t>65 12th main BDS layout</t>
+  </si>
+  <si>
+    <t>abcdef</t>
+  </si>
+  <si>
+    <t>Pass - Customer Registered Successfully!!!</t>
+  </si>
+  <si>
+    <t>22144</t>
+  </si>
+  <si>
+    <t>25093</t>
+  </si>
+  <si>
+    <t>10525</t>
+  </si>
+  <si>
+    <t>Pass - Customer name must not be blank</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Pass - First character can not have space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,7 +958,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,12 +1002,12 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
+      <patternFill patternType="none">
+        <fgColor indexed="52"/>
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
         <fgColor indexed="57"/>
       </patternFill>
     </fill>
@@ -501,17 +1017,27 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="52"/>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="52"/>
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -626,6 +1152,17 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -640,35 +1177,49 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
-      <right style="thin"/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -677,9 +1228,13 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -688,53 +1243,48 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="4" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="5" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="6" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="7" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="8" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="true" applyBorder="true"/>
+  <cellXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -751,10 +1301,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -789,7 +1339,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -824,7 +1374,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -918,21 +1468,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -949,7 +1499,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1001,15 +1551,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -1017,11 +1567,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="51.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="55.5703125" collapsed="true"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="51.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1066,7 +1616,7 @@
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1202,28 +1752,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink display="http://demo.guru99.com/v4/" r:id="rId2" ref="C3:C5"/>
-    <hyperlink display="http://demo.guru99.com/v4/" r:id="rId3" ref="C6:C8"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3:C5" r:id="rId2" display="http://demo.guru99.com/v4/"/>
+    <hyperlink ref="C6:C8" r:id="rId3" display="http://demo.guru99.com/v4/"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="52.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.7109375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1239,7 +1793,7 @@
       <c r="D1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="12" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="3" t="s">
@@ -1281,7 +1835,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
@@ -1305,16 +1859,20 @@
         <v>7771232345</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>131</v>
+        <v>225</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1351,13 +1909,17 @@
         <v>53</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1391,23 +1953,27 @@
         <v>7771237890</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>56</v>
+        <v>226</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
@@ -1417,13 +1983,13 @@
         <v>31855</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I5" s="1">
         <v>237876</v>
@@ -1432,24 +1998,30 @@
         <v>9991237890</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="N5" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>47</v>
@@ -1458,13 +2030,13 @@
         <v>31481</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I6" s="1">
         <v>667897</v>
@@ -1473,21 +2045,27 @@
         <v>5556789087</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="N6" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1">
         <v>12334</v>
@@ -1499,13 +2077,13 @@
         <v>30477</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I7" s="1">
         <v>788767</v>
@@ -1514,12 +2092,14 @@
         <v>5554567897</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M7" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
@@ -1528,10 +2108,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>46</v>
@@ -1540,13 +2120,13 @@
         <v>28690</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="I8" s="1">
         <v>897654</v>
@@ -1555,12 +2135,14 @@
         <v>4448960786</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M8" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
@@ -1569,10 +2151,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>47</v>
@@ -1581,13 +2163,13 @@
         <v>29938</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I9" s="1">
         <v>765897</v>
@@ -1596,12 +2178,14 @@
         <v>4447895432</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M9" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
@@ -1610,20 +2194,20 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="11">
         <v>32527</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>50</v>
@@ -1635,12 +2219,14 @@
         <v>7779081234</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>120</v>
+        <v>227</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M10" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
@@ -1649,20 +2235,20 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>50</v>
@@ -1674,12 +2260,14 @@
         <v>7776892313</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M11" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
@@ -1688,10 +2276,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>47</v>
@@ -1700,7 +2288,7 @@
         <v>235197</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>49</v>
@@ -1715,12 +2303,14 @@
         <v>7771236789</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="M12" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
@@ -1729,19 +2319,39 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="11">
+        <v>31397</v>
+      </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I13" s="1">
+        <v>678543</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2227657890</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
@@ -1750,19 +2360,41 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+        <v>89</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="11">
+        <v>28071</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" s="1">
+        <v>657545</v>
+      </c>
+      <c r="J14" s="1">
+        <v>90167189172</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
     </row>
@@ -1771,19 +2403,41 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="11">
+        <v>32980</v>
+      </c>
+      <c r="F15" s="1">
+        <v>122</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I15" s="1">
+        <v>567987</v>
+      </c>
+      <c r="J15" s="1">
+        <v>8786357718</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
     </row>
@@ -1792,19 +2446,41 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="11">
+        <v>33314</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I16" s="1">
+        <v>657876</v>
+      </c>
+      <c r="J16" s="1">
+        <v>4417678901</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
     </row>
@@ -1813,19 +2489,41 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="11">
+        <v>35964</v>
+      </c>
+      <c r="F17" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I17" s="1">
+        <v>657987</v>
+      </c>
+      <c r="J17" s="1">
+        <v>4417657812</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
     </row>
@@ -1834,19 +2532,38 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="11">
+        <v>34169</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" s="1">
+        <v>786545</v>
+      </c>
+      <c r="J18" s="1">
+        <v>9997863271</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
     </row>
@@ -1855,19 +2572,41 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+        <v>90</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="11">
+        <v>33667</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I19" s="1">
+        <v>879656</v>
+      </c>
+      <c r="J19" s="1">
+        <v>6557891271</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
     </row>
@@ -1876,19 +2615,41 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="11">
+        <v>32238</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G20">
+        <v>56687</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="1">
+        <v>667434</v>
+      </c>
+      <c r="J20" s="1">
+        <v>7779874561</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
@@ -1897,19 +2658,41 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="11">
+        <v>33773</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="1">
+        <v>467543</v>
+      </c>
+      <c r="J21" s="1">
+        <v>7779084515</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
@@ -1918,19 +2701,41 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="11">
+        <v>33437</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="1">
+        <v>786433</v>
+      </c>
+      <c r="J22" s="1">
+        <v>5557789012</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
     </row>
@@ -1939,19 +2744,39 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="11">
+        <v>35859</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="I23" s="1">
+        <v>764367</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1018237829</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
     </row>
@@ -1960,19 +2785,41 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="11">
+        <v>34158</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I24" s="1">
+        <v>775645</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1015677890</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
     </row>
@@ -1981,19 +2828,41 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="11">
+        <v>34432</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H25" s="1">
+        <v>13345</v>
+      </c>
+      <c r="I25" s="1">
+        <v>665745</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1012237893</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
@@ -2002,19 +2871,41 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="11">
+        <v>35163</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I26" s="1">
+        <v>765435</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1016738377</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
     </row>
@@ -2023,19 +2914,41 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="11">
+        <v>32971</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I27" s="1">
+        <v>767546</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1239872361</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
@@ -2044,19 +2957,39 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="11">
+        <v>32975</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>159</v>
+      </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="J28" s="1">
+        <v>4417728910</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
     </row>
@@ -2065,19 +2998,41 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="11">
+        <v>33733</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="J29" s="1">
+        <v>5657811232</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
     </row>
@@ -2086,19 +3041,41 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="11">
+        <v>34095</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J30" s="1">
+        <v>6628725671</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
     </row>
@@ -2107,19 +3084,41 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="11">
+        <v>34888</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J31" s="1">
+        <v>5529874561</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
     </row>
@@ -2128,19 +3127,41 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="11">
+        <v>36025</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I32" s="1">
+        <v>5654325</v>
+      </c>
+      <c r="J32" s="1">
+        <v>5658901234</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
     </row>
@@ -2149,19 +3170,41 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="11">
+        <v>34128</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I33" s="1">
+        <v>5664</v>
+      </c>
+      <c r="J33" s="1">
+        <v>9328982123</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
@@ -2170,19 +3213,39 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="11">
+        <v>34523</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I34" s="1">
+        <v>346765</v>
+      </c>
       <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="K34" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
@@ -2191,19 +3254,41 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="11">
+        <v>35162</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I35" s="1">
+        <v>457865</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
@@ -2212,19 +3297,41 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="11">
+        <v>35977</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="1">
+        <v>778654</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
@@ -2233,19 +3340,41 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="11">
+        <v>34351</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I37" s="1">
+        <v>326787</v>
+      </c>
+      <c r="J37" s="1">
+        <v>5527658765</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
@@ -2254,19 +3383,41 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="11">
+        <v>35527</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I38" s="1">
+        <v>456367</v>
+      </c>
+      <c r="J38" s="1">
+        <v>8806785435</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
@@ -2275,19 +3426,41 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="11">
+        <v>34127</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I39" s="1">
+        <v>235789</v>
+      </c>
+      <c r="J39" s="1">
+        <v>2227658912</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
@@ -2296,19 +3469,41 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="11">
+        <v>34523</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I40" s="1">
+        <v>323678</v>
+      </c>
+      <c r="J40" s="1">
+        <v>2225678901</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>143</v>
+      </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
@@ -2317,19 +3512,41 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
+        <v>94</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="11">
+        <v>35965</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I41" s="1">
+        <v>234878</v>
+      </c>
+      <c r="J41" s="1">
+        <v>4415427819</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
     </row>
@@ -2338,19 +3555,41 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
+        <v>85</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="11">
+        <v>34432</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I42" s="1">
+        <v>879453</v>
+      </c>
+      <c r="J42" s="1">
+        <v>4412568916</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
@@ -2359,19 +3598,41 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43" s="11">
+        <v>32966</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I43" s="1">
+        <v>345788</v>
+      </c>
+      <c r="J43" s="1">
+        <v>5557826541</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
@@ -2380,19 +3641,41 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="11">
+        <v>33333</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I44" s="1">
+        <v>653652</v>
+      </c>
+      <c r="J44" s="1">
+        <v>5554237891</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
@@ -2401,19 +3684,41 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="11">
+        <v>33376</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45" s="1">
+        <v>456456</v>
+      </c>
+      <c r="J45" s="1">
+        <v>90165328917</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
@@ -2424,17 +3729,37 @@
       <c r="B46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="11">
+        <v>35167</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I46" s="1">
+        <v>345235</v>
+      </c>
+      <c r="J46" s="1">
+        <v>8783426621</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
+      <c r="M46" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
@@ -2443,19 +3768,41 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="11">
+        <v>34096</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I47" s="1">
+        <v>765787</v>
+      </c>
+      <c r="J47" s="1">
+        <v>7776528901</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
     </row>
@@ -2464,19 +3811,41 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="11">
+        <v>33708</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I48" s="1">
+        <v>897654</v>
+      </c>
+      <c r="J48" s="1">
+        <v>9992346781</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
     </row>
@@ -2485,19 +3854,41 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="11">
+        <v>31173</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I49" s="1">
+        <v>676588</v>
+      </c>
+      <c r="J49" s="1">
+        <v>2226189271</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
     </row>
@@ -2506,61 +3897,149 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="E50" s="11"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
+      <c r="J50" s="1">
+        <v>1014367829</v>
+      </c>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
+      <c r="M50" s="1" t="s">
+        <v>145</v>
+      </c>
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
     </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J51" s="14"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="K2"/>
-    <hyperlink r:id="rId2" ref="K3"/>
-    <hyperlink r:id="rId3" ref="K4"/>
-    <hyperlink r:id="rId4" ref="K5"/>
-    <hyperlink r:id="rId5" ref="K6"/>
-    <hyperlink r:id="rId6" ref="K7"/>
-    <hyperlink r:id="rId7" ref="K8"/>
-    <hyperlink r:id="rId8" ref="K9"/>
-    <hyperlink r:id="rId9" ref="K10"/>
-    <hyperlink r:id="rId10" ref="K11"/>
-    <hyperlink r:id="rId11" ref="K12"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K4" r:id="rId3"/>
+    <hyperlink ref="K5" r:id="rId4"/>
+    <hyperlink ref="K6" r:id="rId5"/>
+    <hyperlink ref="K7" r:id="rId6"/>
+    <hyperlink ref="K8" r:id="rId7"/>
+    <hyperlink ref="K9" r:id="rId8"/>
+    <hyperlink ref="K10" r:id="rId9"/>
+    <hyperlink ref="K11" r:id="rId10"/>
+    <hyperlink ref="K12" r:id="rId11"/>
+    <hyperlink ref="K13" r:id="rId12"/>
+    <hyperlink ref="K14" r:id="rId13"/>
+    <hyperlink ref="K15" r:id="rId14"/>
+    <hyperlink ref="K16" r:id="rId15"/>
+    <hyperlink ref="K17" r:id="rId16"/>
+    <hyperlink ref="K18" r:id="rId17"/>
+    <hyperlink ref="L47" r:id="rId18"/>
+    <hyperlink ref="K19" r:id="rId19"/>
+    <hyperlink ref="K20" r:id="rId20"/>
+    <hyperlink ref="K21" r:id="rId21"/>
+    <hyperlink ref="K22" r:id="rId22"/>
+    <hyperlink ref="K23" r:id="rId23"/>
+    <hyperlink ref="K24" r:id="rId24"/>
+    <hyperlink ref="K25" r:id="rId25"/>
+    <hyperlink ref="K26" r:id="rId26"/>
+    <hyperlink ref="K27" r:id="rId27"/>
+    <hyperlink ref="K28" r:id="rId28"/>
+    <hyperlink ref="K29" r:id="rId29"/>
+    <hyperlink ref="K30" r:id="rId30"/>
+    <hyperlink ref="K31" r:id="rId31"/>
+    <hyperlink ref="K32" r:id="rId32"/>
+    <hyperlink ref="K33" r:id="rId33"/>
+    <hyperlink ref="K34" r:id="rId34"/>
+    <hyperlink ref="K35" r:id="rId35"/>
+    <hyperlink ref="K36" r:id="rId36"/>
+    <hyperlink ref="K37" r:id="rId37"/>
+    <hyperlink ref="K38" r:id="rId38"/>
+    <hyperlink ref="K39" r:id="rId39"/>
+    <hyperlink ref="K40" r:id="rId40"/>
+    <hyperlink ref="K41" r:id="rId41"/>
+    <hyperlink ref="K42" r:id="rId42"/>
+    <hyperlink ref="K43" r:id="rId43"/>
+    <hyperlink ref="K44" r:id="rId44"/>
+    <hyperlink ref="K45" r:id="rId45"/>
+    <hyperlink ref="K46" r:id="rId46"/>
+    <hyperlink ref="K47" r:id="rId47"/>
+    <hyperlink ref="K48" r:id="rId48"/>
+    <hyperlink ref="K49" r:id="rId49"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="0" r:id="rId12"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H8:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="8" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="10" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f>LEN(H9)</f>
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AddNewCustInfo changes completed DeleteCustInfo changes WIP
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="NewCust" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="EditCust" sheetId="3" r:id="rId4"/>
-    <sheet name="DeleteCust" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="EditCust" sheetId="3" r:id="rId3"/>
+    <sheet name="DeleteCust" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NewCust!$H$1:$H$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NewCust!$H$1:$H$51</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="312">
   <si>
     <t>testcaseID</t>
   </si>
@@ -188,9 +187,6 @@
     <t>Mysore</t>
   </si>
   <si>
-    <t>jim@test.com</t>
-  </si>
-  <si>
     <t>54 7th main DR road</t>
   </si>
   <si>
@@ -317,9 +313,6 @@
     <t>Only spaces in password</t>
   </si>
   <si>
-    <t>Email id exceeding 10 characters</t>
-  </si>
-  <si>
     <t>Password exceeding 10 characters</t>
   </si>
   <si>
@@ -464,11 +457,6 @@
     <t>Email-ID is not valid</t>
   </si>
   <si>
-    <t xml:space="preserve">Customer name must not be blankDate Field must not be blankAddress Field must not be blank
-City Field must not be blankState must not be blankPIN Code must not be blankMobile no must not be blankEmail-ID must not be blankPassword must not be blank
-</t>
-  </si>
-  <si>
     <t>Om</t>
   </si>
   <si>
@@ -655,9 +643,6 @@
     <t>anu@test.com</t>
   </si>
   <si>
-    <t>san@test.com</t>
-  </si>
-  <si>
     <t>pam@test.com</t>
   </si>
   <si>
@@ -670,33 +655,12 @@
     <t>han@test.com</t>
   </si>
   <si>
-    <t>kir@test.com</t>
-  </si>
-  <si>
     <t>neh@test.com</t>
   </si>
   <si>
     <t>lai@test.com</t>
   </si>
   <si>
-    <t>bin@test.com</t>
-  </si>
-  <si>
-    <t>ron@test.com</t>
-  </si>
-  <si>
-    <t>roo@test.com</t>
-  </si>
-  <si>
-    <t>vee@test.com</t>
-  </si>
-  <si>
-    <t>dar@test.com</t>
-  </si>
-  <si>
-    <t>ali@test.com</t>
-  </si>
-  <si>
     <t>ano@test.com</t>
   </si>
   <si>
@@ -709,9 +673,6 @@
     <t>jos@test.com</t>
   </si>
   <si>
-    <t>kei@test.com</t>
-  </si>
-  <si>
     <t>moh@test.com</t>
   </si>
   <si>
@@ -742,9 +703,6 @@
     <t>Madhya Pradesh</t>
   </si>
   <si>
-    <t>Madurai</t>
-  </si>
-  <si>
     <t>Salem</t>
   </si>
   <si>
@@ -916,32 +874,101 @@
     <t>abcdef</t>
   </si>
   <si>
+    <t>jim1@test.com</t>
+  </si>
+  <si>
+    <t>keit@test.com</t>
+  </si>
+  <si>
     <t>Pass - Customer Registered Successfully!!!</t>
   </si>
   <si>
-    <t>22144</t>
-  </si>
-  <si>
-    <t>25093</t>
-  </si>
-  <si>
-    <t>10525</t>
-  </si>
-  <si>
-    <t>Pass - Customer name must not be blank</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>Pass - First character can not have space</t>
+    <t>Existing email id</t>
+  </si>
+  <si>
+    <t>Jilka</t>
+  </si>
+  <si>
+    <t>544 8th main GKV road</t>
+  </si>
+  <si>
+    <t>sanya@test.com</t>
+  </si>
+  <si>
+    <t>Email Address Already Exist !!</t>
+  </si>
+  <si>
+    <t>Customer name must not be blankDate Field must not be blankAddress Field must not be blankCity Field must not be blankState must not be blankPIN Code must not be blankMobile no must not be blankEmail-ID must not be blankPassword must not be blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 </t>
+  </si>
+  <si>
+    <t>rootest.com</t>
+  </si>
+  <si>
+    <t>vee@test</t>
+  </si>
+  <si>
+    <t>dar</t>
+  </si>
+  <si>
+    <t>^&amp;*%%&amp;*</t>
+  </si>
+  <si>
+    <t>kiran@test.com</t>
+  </si>
+  <si>
+    <t>Email id exceeding 30 characters</t>
+  </si>
+  <si>
+    <t>ali12345678901234562@test.com11</t>
+  </si>
+  <si>
+    <t>Do you really want to delete this Customer?</t>
+  </si>
+  <si>
+    <t>Customer deleted Successfully</t>
+  </si>
+  <si>
+    <t>Customer does not exist!!</t>
+  </si>
+  <si>
+    <t>Existing customer id</t>
+  </si>
+  <si>
+    <t>Pass - Customer deleted Successfully</t>
+  </si>
+  <si>
+    <t>Fail - Customer does not exist!!</t>
+  </si>
+  <si>
+    <t>Customer ID is required</t>
+  </si>
+  <si>
+    <t>Blank customer id</t>
+  </si>
+  <si>
+    <t>Pass - Customer ID is required</t>
+  </si>
+  <si>
+    <t>91875</t>
+  </si>
+  <si>
+    <t>53403</t>
+  </si>
+  <si>
+    <t>Fail - Message mismatch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -957,8 +984,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -969,6 +1003,117 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
       </patternFill>
     </fill>
     <fill>
@@ -1028,16 +1173,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
+        <fgColor indexed="52"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="71">
     <border>
       <left/>
       <right/>
@@ -1189,6 +1329,840 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1256,7 +2230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1272,12 +2246,77 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="37" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="41" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="65" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="69" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1562,7 +2601,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,7 +2655,7 @@
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="82" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1763,17 +2802,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O51" sqref="N4:O51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="52.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="10.7109375" style="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="66.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1835,7 +2874,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>47</v>
@@ -1859,19 +2898,19 @@
         <v>7771232345</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>295</v>
+      <c r="N2" s="81" t="s">
+        <v>309</v>
+      </c>
+      <c r="O2" s="81" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1906,19 +2945,19 @@
         <v>7778907689</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>53</v>
+        <v>282</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>295</v>
+      <c r="N3" s="84" t="s">
+        <v>310</v>
+      </c>
+      <c r="O3" s="84" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1938,10 +2977,10 @@
         <v>28921</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>50</v>
@@ -1953,27 +2992,23 @@
         <v>7771237890</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>226</v>
+        <v>283</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>295</v>
-      </c>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
@@ -1983,13 +3018,13 @@
         <v>31855</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I5" s="1">
         <v>237876</v>
@@ -1998,30 +3033,26 @@
         <v>9991237890</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>300</v>
-      </c>
-      <c r="O5" s="19" t="s">
-        <v>299</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>47</v>
@@ -2030,13 +3061,13 @@
         <v>31481</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I6" s="1">
         <v>667897</v>
@@ -2045,27 +3076,23 @@
         <v>5556789087</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="O6" s="20" t="s">
-        <v>301</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="N6" s="85"/>
+      <c r="O6" s="85"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>12334</v>
@@ -2077,13 +3104,13 @@
         <v>30477</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I7" s="1">
         <v>788767</v>
@@ -2092,26 +3119,26 @@
         <v>5554567897</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="N7" s="85"/>
+      <c r="O7" s="85"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>46</v>
@@ -2120,13 +3147,13 @@
         <v>28690</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="I8" s="1">
         <v>897654</v>
@@ -2135,26 +3162,26 @@
         <v>4448960786</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="N8" s="85"/>
+      <c r="O8" s="85"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>47</v>
@@ -2163,13 +3190,13 @@
         <v>29938</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I9" s="1">
         <v>765897</v>
@@ -2178,36 +3205,36 @@
         <v>4447895432</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="85"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="11">
         <v>32527</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>50</v>
@@ -2219,36 +3246,36 @@
         <v>7779081234</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="L10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="N10" s="85"/>
+      <c r="O10" s="85"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>50</v>
@@ -2260,26 +3287,26 @@
         <v>7776892313</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="N11" s="85"/>
+      <c r="O11" s="85"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>47</v>
@@ -2288,7 +3315,7 @@
         <v>235197</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>49</v>
@@ -2303,26 +3330,26 @@
         <v>7771236789</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
+      <c r="N12" s="85"/>
+      <c r="O12" s="85"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>46</v>
@@ -2332,10 +3359,10 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I13" s="1">
         <v>678543</v>
@@ -2344,26 +3371,26 @@
         <v>2227657890</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+        <v>133</v>
+      </c>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>47</v>
@@ -2372,13 +3399,13 @@
         <v>28071</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I14" s="1">
         <v>657545</v>
@@ -2387,26 +3414,26 @@
         <v>90167189172</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N14" s="85"/>
+      <c r="O14" s="85"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>46</v>
@@ -2418,10 +3445,10 @@
         <v>122</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I15" s="1">
         <v>567987</v>
@@ -2430,26 +3457,26 @@
         <v>8786357718</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="N15" s="85"/>
+      <c r="O15" s="85"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>47</v>
@@ -2458,13 +3485,13 @@
         <v>33314</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I16" s="1">
         <v>657876</v>
@@ -2473,26 +3500,26 @@
         <v>4417678901</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="N16" s="85"/>
+      <c r="O16" s="85"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>47</v>
@@ -2500,14 +3527,14 @@
       <c r="E17" s="11">
         <v>35964</v>
       </c>
-      <c r="F17" t="s">
-        <v>161</v>
+      <c r="F17" s="1" t="s">
+        <v>158</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I17" s="1">
         <v>657987</v>
@@ -2516,26 +3543,26 @@
         <v>4417657812</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="L17" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="85"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>47</v>
@@ -2544,10 +3571,11 @@
         <v>34169</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>100</v>
+        <v>222</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="15" t="s">
+        <v>98</v>
       </c>
       <c r="I18" s="1">
         <v>786545</v>
@@ -2556,26 +3584,26 @@
         <v>9997863271</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="N18" s="85"/>
+      <c r="O18" s="85"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>46</v>
@@ -2584,13 +3612,13 @@
         <v>33667</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="I19" s="1">
         <v>879656</v>
@@ -2599,26 +3627,26 @@
         <v>6557891271</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N19" s="85"/>
+      <c r="O19" s="85"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>46</v>
@@ -2627,9 +3655,9 @@
         <v>32238</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="G20">
+        <v>254</v>
+      </c>
+      <c r="G20" s="1">
         <v>56687</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -2642,26 +3670,26 @@
         <v>7779874561</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="N20" s="85"/>
+      <c r="O20" s="85"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>46</v>
@@ -2670,10 +3698,10 @@
         <v>33773</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>50</v>
@@ -2685,26 +3713,26 @@
         <v>7779084515</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M21" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="N21" s="85"/>
+      <c r="O21" s="85"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>46</v>
@@ -2713,13 +3741,13 @@
         <v>33437</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I22" s="1">
         <v>786433</v>
@@ -2728,26 +3756,26 @@
         <v>5557789012</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="L22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="N22" s="85"/>
+      <c r="O22" s="85"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>46</v>
@@ -2756,10 +3784,10 @@
         <v>35859</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1">
@@ -2769,26 +3797,26 @@
         <v>1018237829</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
+        <v>136</v>
+      </c>
+      <c r="N23" s="85"/>
+      <c r="O23" s="85"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>46</v>
@@ -2797,13 +3825,13 @@
         <v>34158</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="I24" s="1">
         <v>775645</v>
@@ -2812,26 +3840,26 @@
         <v>1015677890</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N24" s="85"/>
+      <c r="O24" s="85"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>46</v>
@@ -2840,10 +3868,10 @@
         <v>34432</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="H25" s="1">
         <v>13345</v>
@@ -2855,26 +3883,26 @@
         <v>1012237893</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="N25" s="85"/>
+      <c r="O25" s="85"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>47</v>
@@ -2883,13 +3911,13 @@
         <v>35163</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="I26" s="1">
         <v>765435</v>
@@ -2898,26 +3926,26 @@
         <v>1016738377</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="N26" s="85"/>
+      <c r="O26" s="85"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>46</v>
@@ -2926,13 +3954,13 @@
         <v>32971</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="I27" s="1">
         <v>767546</v>
@@ -2941,26 +3969,26 @@
         <v>1239872361</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="L27" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M27" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M27" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
+      <c r="N27" s="85"/>
+      <c r="O27" s="85"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>46</v>
@@ -2969,39 +3997,39 @@
         <v>32975</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1">
         <v>4417728910</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
+        <v>137</v>
+      </c>
+      <c r="N28" s="85"/>
+      <c r="O28" s="85"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>47</v>
@@ -3010,41 +4038,41 @@
         <v>33733</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="J29" s="1">
         <v>5657811232</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N29" s="85"/>
+      <c r="O29" s="85"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>46</v>
@@ -3053,41 +4081,41 @@
         <v>34095</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="J30" s="1">
         <v>6628725671</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="N30" s="85"/>
+      <c r="O30" s="85"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>47</v>
@@ -3096,41 +4124,41 @@
         <v>34888</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="J31" s="1">
         <v>5529874561</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="N31" s="85"/>
+      <c r="O31" s="85"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>47</v>
@@ -3139,13 +4167,13 @@
         <v>36025</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="I32" s="1">
         <v>5654325</v>
@@ -3154,26 +4182,26 @@
         <v>5658901234</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>208</v>
+        <v>289</v>
       </c>
       <c r="L32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
+      <c r="N32" s="85"/>
+      <c r="O32" s="85"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>47</v>
@@ -3182,13 +4210,13 @@
         <v>34128</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="I33" s="1">
         <v>5664</v>
@@ -3197,26 +4225,26 @@
         <v>9328982123</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="N33" s="85"/>
+      <c r="O33" s="85"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>47</v>
@@ -3225,10 +4253,10 @@
         <v>34523</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>50</v>
@@ -3238,26 +4266,26 @@
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
+        <v>140</v>
+      </c>
+      <c r="N34" s="85"/>
+      <c r="O34" s="85"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>47</v>
@@ -3266,7 +4294,7 @@
         <v>35162</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>49</v>
@@ -3278,29 +4306,29 @@
         <v>457865</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N35" s="85"/>
+      <c r="O35" s="85"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>47</v>
@@ -3309,10 +4337,10 @@
         <v>35977</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>50</v>
@@ -3321,29 +4349,29 @@
         <v>778654</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
+        <v>138</v>
+      </c>
+      <c r="N36" s="85"/>
+      <c r="O36" s="85"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>46</v>
@@ -3352,41 +4380,41 @@
         <v>34351</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="I37" s="1">
         <v>326787</v>
       </c>
-      <c r="J37" s="1">
-        <v>5527658765</v>
+      <c r="J37" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>213</v>
+        <v>297</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="N37" s="85"/>
+      <c r="O37" s="85"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>47</v>
@@ -3395,13 +4423,13 @@
         <v>35527</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="I38" s="1">
         <v>456367</v>
@@ -3410,26 +4438,26 @@
         <v>8806785435</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="L38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
+      <c r="N38" s="85"/>
+      <c r="O38" s="85"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>47</v>
@@ -3438,13 +4466,13 @@
         <v>34127</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I39" s="1">
         <v>235789</v>
@@ -3453,26 +4481,26 @@
         <v>2227658912</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="L39" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="M39" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="85"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>46</v>
@@ -3481,13 +4509,13 @@
         <v>34523</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I40" s="1">
         <v>323678</v>
@@ -3495,27 +4523,25 @@
       <c r="J40" s="1">
         <v>2225678901</v>
       </c>
-      <c r="K40" s="2" t="s">
-        <v>216</v>
-      </c>
+      <c r="K40" s="2"/>
       <c r="L40" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
+        <v>141</v>
+      </c>
+      <c r="N40" s="85"/>
+      <c r="O40" s="85"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>47</v>
@@ -3524,13 +4550,13 @@
         <v>35965</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I41" s="1">
         <v>234878</v>
@@ -3538,27 +4564,27 @@
       <c r="J41" s="1">
         <v>4415427819</v>
       </c>
-      <c r="K41" s="2" t="s">
-        <v>217</v>
+      <c r="K41" s="16" t="s">
+        <v>292</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="N41" s="85"/>
+      <c r="O41" s="85"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>47</v>
@@ -3567,13 +4593,13 @@
         <v>34432</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I42" s="1">
         <v>879453</v>
@@ -3582,26 +4608,26 @@
         <v>4412568916</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>218</v>
+        <v>293</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="N42" s="85"/>
+      <c r="O42" s="85"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>46</v>
@@ -3610,13 +4636,13 @@
         <v>32966</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I43" s="1">
         <v>345788</v>
@@ -3625,26 +4651,26 @@
         <v>5557826541</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>219</v>
+        <v>294</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="N43" s="85"/>
+      <c r="O43" s="85"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>46</v>
@@ -3653,13 +4679,13 @@
         <v>33333</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I44" s="1">
         <v>653652</v>
@@ -3668,257 +4694,299 @@
         <v>5554237891</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
+        <v>142</v>
+      </c>
+      <c r="N44" s="85"/>
+      <c r="O44" s="85"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>96</v>
+        <v>286</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>189</v>
+        <v>287</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E45" s="11">
-        <v>33376</v>
+        <v>34108</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="I45" s="1">
-        <v>456456</v>
+        <v>453245</v>
       </c>
       <c r="J45" s="1">
-        <v>90165328917</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>221</v>
+        <v>2227893421</v>
+      </c>
+      <c r="K45" s="2" t="str">
+        <f>K2</f>
+        <v>jos@test.com</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
+        <v>290</v>
+      </c>
+      <c r="N45" s="85"/>
+      <c r="O45" s="85"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>22</v>
+        <v>298</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E46" s="11">
-        <v>35167</v>
+        <v>33376</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I46" s="1">
-        <v>345235</v>
+        <v>456456</v>
       </c>
       <c r="J46" s="1">
-        <v>8783426621</v>
+        <v>90165328917</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="L46" s="1"/>
+        <v>299</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="M46" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="N46" s="85"/>
+      <c r="O46" s="85"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>98</v>
+        <v>22</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E47" s="11">
-        <v>34096</v>
+        <v>35167</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="I47" s="1">
-        <v>765787</v>
+        <v>345235</v>
       </c>
       <c r="J47" s="1">
-        <v>7776528901</v>
+        <v>8783426621</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>193</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="L47" s="1"/>
       <c r="M47" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="N47" s="85"/>
+      <c r="O47" s="85"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E48" s="11">
-        <v>33708</v>
+        <v>34096</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I48" s="1">
-        <v>897654</v>
+        <v>765787</v>
       </c>
       <c r="J48" s="1">
-        <v>9992346781</v>
+        <v>7776528901</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>194</v>
+        <v>212</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="N48" s="85"/>
+      <c r="O48" s="85"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E49" s="11">
-        <v>31173</v>
+        <v>33708</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>147</v>
+        <v>251</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>235</v>
+        <v>98</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="I49" s="1">
-        <v>676588</v>
+        <v>897654</v>
       </c>
       <c r="J49" s="1">
-        <v>2226189271</v>
+        <v>9992346781</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>261</v>
+        <v>213</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="N49" s="85"/>
+      <c r="O49" s="85"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+        <v>95</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E50" s="11">
+        <v>31173</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I50" s="1">
+        <v>676588</v>
+      </c>
       <c r="J50" s="1">
-        <v>1014367829</v>
-      </c>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
+        <v>2226189271</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>192</v>
+      </c>
       <c r="M50" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="N50" s="85"/>
+      <c r="O50" s="85"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J51" s="14"/>
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="N51" s="85"/>
+      <c r="O51" s="85"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J52" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3939,7 +5007,7 @@
     <hyperlink ref="K16" r:id="rId15"/>
     <hyperlink ref="K17" r:id="rId16"/>
     <hyperlink ref="K18" r:id="rId17"/>
-    <hyperlink ref="L47" r:id="rId18"/>
+    <hyperlink ref="L48" r:id="rId18"/>
     <hyperlink ref="K19" r:id="rId19"/>
     <hyperlink ref="K20" r:id="rId20"/>
     <hyperlink ref="K21" r:id="rId21"/>
@@ -3961,54 +5029,22 @@
     <hyperlink ref="K37" r:id="rId37"/>
     <hyperlink ref="K38" r:id="rId38"/>
     <hyperlink ref="K39" r:id="rId39"/>
-    <hyperlink ref="K40" r:id="rId40"/>
-    <hyperlink ref="K41" r:id="rId41"/>
-    <hyperlink ref="K42" r:id="rId42"/>
-    <hyperlink ref="K43" r:id="rId43"/>
-    <hyperlink ref="K44" r:id="rId44"/>
-    <hyperlink ref="K45" r:id="rId45"/>
-    <hyperlink ref="K46" r:id="rId46"/>
-    <hyperlink ref="K47" r:id="rId47"/>
-    <hyperlink ref="K48" r:id="rId48"/>
-    <hyperlink ref="K49" r:id="rId49"/>
+    <hyperlink ref="K42" r:id="rId40" display="roo@test.com"/>
+    <hyperlink ref="K43" r:id="rId41"/>
+    <hyperlink ref="K44" r:id="rId42" display="dar@test.com"/>
+    <hyperlink ref="K46" r:id="rId43"/>
+    <hyperlink ref="K47" r:id="rId44"/>
+    <hyperlink ref="K48" r:id="rId45"/>
+    <hyperlink ref="K49" r:id="rId46"/>
+    <hyperlink ref="K50" r:id="rId47"/>
+    <hyperlink ref="K45" r:id="rId48" display="kei@test.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId50"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H8:H10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="8" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H8" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H9" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H10">
-        <f>LEN(H9)</f>
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4020,26 +5056,564 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="56" t="s">
+        <v>310</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E6" s="60" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E9" s="63" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E11" s="65" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E12" s="66" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E14" s="68" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E15" s="69" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E16" s="70" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E17" s="71" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E19" s="73" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E20" s="74" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="75">
+        <v>20</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="75" t="s">
+        <v>301</v>
+      </c>
+      <c r="E21" s="78" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E22" s="79" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="77">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E23" s="80" t="s">
+        <v>308</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="9.140625" style="31" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="17">
+        <v>43455</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="18">
+        <v>39551</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="19">
+        <v>25023</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="19">
+        <v>99287</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="19">
+        <v>44146</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="19">
+        <v>55287</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="32">
+        <v>6671</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="20">
+        <v>88191</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="21">
+        <v>98587</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="33">
+        <v>52092</v>
+      </c>
+      <c r="I12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="22">
+        <v>6680</v>
+      </c>
+      <c r="I13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="34">
+        <v>91806</v>
+      </c>
+      <c r="I14" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="35">
+        <v>6453</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="36">
+        <v>83119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="37">
+        <v>98074</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="23">
+        <v>69389</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="24">
+        <v>51934</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="25">
+        <v>35485</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="26">
+        <v>36131</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="27">
+        <v>25974</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="28">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="29">
+        <v>86818</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="30">
+        <v>4904</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="38" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="39" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="40" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="41" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="42" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="43" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="44" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="45" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="46" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="47" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="48" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="49" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="50" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="51" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="52" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="53" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="54" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="55" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Writing cust id into delete sheet after adding. Clearing excel data after delete WIP
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NewCust!$H$1:$H$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NewCust!$M$1:$M$52</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="319">
   <si>
     <t>testcaseID</t>
   </si>
@@ -880,88 +880,109 @@
     <t>keit@test.com</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
+    <t>Existing email id</t>
+  </si>
+  <si>
+    <t>Jilka</t>
+  </si>
+  <si>
+    <t>544 8th main GKV road</t>
+  </si>
+  <si>
+    <t>sanya@test.com</t>
+  </si>
+  <si>
+    <t>Email Address Already Exist !!</t>
+  </si>
+  <si>
+    <t>Customer name must not be blankDate Field must not be blankAddress Field must not be blankCity Field must not be blankState must not be blankPIN Code must not be blankMobile no must not be blankEmail-ID must not be blankPassword must not be blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 </t>
+  </si>
+  <si>
+    <t>rootest.com</t>
+  </si>
+  <si>
+    <t>vee@test</t>
+  </si>
+  <si>
+    <t>dar</t>
+  </si>
+  <si>
+    <t>^&amp;*%%&amp;*</t>
+  </si>
+  <si>
+    <t>kiran@test.com</t>
+  </si>
+  <si>
+    <t>Email id exceeding 30 characters</t>
+  </si>
+  <si>
+    <t>ali12345678901234562@test.com11</t>
+  </si>
+  <si>
+    <t>Do you really want to delete this Customer?</t>
+  </si>
+  <si>
+    <t>Customer deleted Successfully</t>
+  </si>
+  <si>
+    <t>Customer does not exist!!</t>
+  </si>
+  <si>
+    <t>Existing customer id</t>
+  </si>
+  <si>
+    <t>Customer ID is required</t>
+  </si>
+  <si>
+    <t>Blank customer id</t>
+  </si>
+  <si>
+    <t>You are not authorize to delete this customer!!</t>
+  </si>
+  <si>
+    <t>Only spaces in customer id</t>
+  </si>
+  <si>
+    <t>Characters in customer id</t>
+  </si>
+  <si>
+    <t>Special characters in customer id</t>
+  </si>
+  <si>
+    <t>Non existing customer id</t>
+  </si>
+  <si>
+    <t>Previously deleted customer id</t>
+  </si>
+  <si>
+    <t>Customer id exceeding 10 digits(Generated ids are &lt;10 digits as of now, hence non existing 11 digits customer id is used for testing)</t>
+  </si>
+  <si>
+    <t>customerid</t>
+  </si>
+  <si>
+    <t>$%*(^%$</t>
+  </si>
+  <si>
     <t>Pass - Customer Registered Successfully!!!</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>Existing email id</t>
-  </si>
-  <si>
-    <t>Jilka</t>
-  </si>
-  <si>
-    <t>544 8th main GKV road</t>
-  </si>
-  <si>
-    <t>sanya@test.com</t>
-  </si>
-  <si>
-    <t>Email Address Already Exist !!</t>
-  </si>
-  <si>
-    <t>Customer name must not be blankDate Field must not be blankAddress Field must not be blankCity Field must not be blankState must not be blankPIN Code must not be blankMobile no must not be blankEmail-ID must not be blankPassword must not be blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 </t>
-  </si>
-  <si>
-    <t>rootest.com</t>
-  </si>
-  <si>
-    <t>vee@test</t>
-  </si>
-  <si>
-    <t>dar</t>
-  </si>
-  <si>
-    <t>^&amp;*%%&amp;*</t>
-  </si>
-  <si>
-    <t>kiran@test.com</t>
-  </si>
-  <si>
-    <t>Email id exceeding 30 characters</t>
-  </si>
-  <si>
-    <t>ali12345678901234562@test.com11</t>
-  </si>
-  <si>
-    <t>Do you really want to delete this Customer?</t>
-  </si>
-  <si>
-    <t>Customer deleted Successfully</t>
-  </si>
-  <si>
-    <t>Customer does not exist!!</t>
-  </si>
-  <si>
-    <t>Existing customer id</t>
+    <t>94493</t>
+  </si>
+  <si>
+    <t>45887</t>
+  </si>
+  <si>
+    <t>56120</t>
   </si>
   <si>
     <t>Pass - Customer deleted Successfully</t>
-  </si>
-  <si>
-    <t>Fail - Customer does not exist!!</t>
-  </si>
-  <si>
-    <t>Customer ID is required</t>
-  </si>
-  <si>
-    <t>Blank customer id</t>
-  </si>
-  <si>
-    <t>Pass - Customer ID is required</t>
-  </si>
-  <si>
-    <t>91875</t>
-  </si>
-  <si>
-    <t>53403</t>
-  </si>
-  <si>
-    <t>Fail - Message mismatch</t>
   </si>
 </sst>
 </file>
@@ -992,7 +1013,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1047,17 +1068,7 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
+      <patternFill patternType="none">
         <fgColor indexed="52"/>
       </patternFill>
     </fill>
@@ -1096,88 +1107,8 @@
         <fgColor indexed="57"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="71">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1974,263 +1905,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2288,35 +1968,20 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="60" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="61" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="62" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="64" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="65" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="69" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="70" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="66" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2655,7 +2320,7 @@
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="82" t="s">
+      <c r="G2" s="62" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2804,8 +2469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O51" sqref="N4:O51"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,11 +2571,11 @@
       <c r="M2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="81" t="s">
-        <v>309</v>
-      </c>
-      <c r="O2" s="81" t="s">
-        <v>284</v>
+      <c r="N2" s="63" t="s">
+        <v>315</v>
+      </c>
+      <c r="O2" s="63" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2953,11 +2618,11 @@
       <c r="M3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N3" s="84" t="s">
-        <v>310</v>
-      </c>
-      <c r="O3" s="84" t="s">
-        <v>284</v>
+      <c r="N3" s="64" t="s">
+        <v>316</v>
+      </c>
+      <c r="O3" s="64" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -3000,8 +2665,12 @@
       <c r="M4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
+      <c r="N4" s="65" t="s">
+        <v>317</v>
+      </c>
+      <c r="O4" s="65" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -3041,8 +2710,8 @@
       <c r="M5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -3084,8 +2753,8 @@
       <c r="M6" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N6" s="85"/>
-      <c r="O6" s="85"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -3127,8 +2796,8 @@
       <c r="M7" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -3170,8 +2839,8 @@
       <c r="M8" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -3213,8 +2882,8 @@
       <c r="M9" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
+      <c r="N9" s="58"/>
+      <c r="O9" s="58"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -3254,8 +2923,8 @@
       <c r="M10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N10" s="85"/>
-      <c r="O10" s="85"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="58"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -3295,8 +2964,8 @@
       <c r="M11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="N11" s="85"/>
-      <c r="O11" s="85"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -3338,8 +3007,8 @@
       <c r="M12" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N12" s="85"/>
-      <c r="O12" s="85"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -3379,8 +3048,8 @@
       <c r="M13" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -3422,8 +3091,8 @@
       <c r="M14" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -3465,8 +3134,8 @@
       <c r="M15" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N15" s="85"/>
-      <c r="O15" s="85"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -3508,8 +3177,8 @@
       <c r="M16" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85"/>
+      <c r="N16" s="58"/>
+      <c r="O16" s="58"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -3551,8 +3220,8 @@
       <c r="M17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N17" s="85"/>
-      <c r="O17" s="85"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="58"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -3592,8 +3261,8 @@
       <c r="M18" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="N18" s="85"/>
-      <c r="O18" s="85"/>
+      <c r="N18" s="58"/>
+      <c r="O18" s="58"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -3635,8 +3304,8 @@
       <c r="M19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
+      <c r="N19" s="58"/>
+      <c r="O19" s="58"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
@@ -3678,8 +3347,8 @@
       <c r="M20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N20" s="85"/>
-      <c r="O20" s="85"/>
+      <c r="N20" s="58"/>
+      <c r="O20" s="58"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -3721,8 +3390,8 @@
       <c r="M21" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N21" s="85"/>
-      <c r="O21" s="85"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="58"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
@@ -3764,8 +3433,8 @@
       <c r="M22" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N22" s="85"/>
-      <c r="O22" s="85"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="58"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -3805,8 +3474,8 @@
       <c r="M23" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="N23" s="85"/>
-      <c r="O23" s="85"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
@@ -3848,8 +3517,8 @@
       <c r="M24" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N24" s="85"/>
-      <c r="O24" s="85"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="58"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
@@ -3891,8 +3560,8 @@
       <c r="M25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N25" s="85"/>
-      <c r="O25" s="85"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="58"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -3934,8 +3603,8 @@
       <c r="M26" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N26" s="85"/>
-      <c r="O26" s="85"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="58"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
@@ -3977,8 +3646,8 @@
       <c r="M27" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N27" s="85"/>
-      <c r="O27" s="85"/>
+      <c r="N27" s="58"/>
+      <c r="O27" s="58"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -4018,8 +3687,8 @@
       <c r="M28" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="N28" s="85"/>
-      <c r="O28" s="85"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
@@ -4061,8 +3730,8 @@
       <c r="M29" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N29" s="85"/>
-      <c r="O29" s="85"/>
+      <c r="N29" s="58"/>
+      <c r="O29" s="58"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
@@ -4104,8 +3773,8 @@
       <c r="M30" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="N30" s="85"/>
-      <c r="O30" s="85"/>
+      <c r="N30" s="58"/>
+      <c r="O30" s="58"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
@@ -4147,8 +3816,8 @@
       <c r="M31" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N31" s="85"/>
-      <c r="O31" s="85"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
@@ -4182,7 +3851,7 @@
         <v>5658901234</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>122</v>
@@ -4190,8 +3859,8 @@
       <c r="M32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N32" s="85"/>
-      <c r="O32" s="85"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="58"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
@@ -4233,8 +3902,8 @@
       <c r="M33" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="N33" s="85"/>
-      <c r="O33" s="85"/>
+      <c r="N33" s="58"/>
+      <c r="O33" s="58"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -4274,8 +3943,8 @@
       <c r="M34" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="N34" s="85"/>
-      <c r="O34" s="85"/>
+      <c r="N34" s="58"/>
+      <c r="O34" s="58"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
@@ -4317,8 +3986,8 @@
       <c r="M35" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N35" s="85"/>
-      <c r="O35" s="85"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="58"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
@@ -4360,8 +4029,8 @@
       <c r="M36" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="N36" s="85"/>
-      <c r="O36" s="85"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="58"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
@@ -4392,10 +4061,10 @@
         <v>326787</v>
       </c>
       <c r="J37" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>297</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>122</v>
@@ -4403,8 +4072,8 @@
       <c r="M37" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N37" s="85"/>
-      <c r="O37" s="85"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
@@ -4446,8 +4115,8 @@
       <c r="M38" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N38" s="85"/>
-      <c r="O38" s="85"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -4489,8 +4158,8 @@
       <c r="M39" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N39" s="85"/>
-      <c r="O39" s="85"/>
+      <c r="N39" s="58"/>
+      <c r="O39" s="58"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
@@ -4530,8 +4199,8 @@
       <c r="M40" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="N40" s="85"/>
-      <c r="O40" s="85"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="58"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -4565,7 +4234,7 @@
         <v>4415427819</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>122</v>
@@ -4573,8 +4242,8 @@
       <c r="M41" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N41" s="85"/>
-      <c r="O41" s="85"/>
+      <c r="N41" s="58"/>
+      <c r="O41" s="58"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -4608,7 +4277,7 @@
         <v>4412568916</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>122</v>
@@ -4616,8 +4285,8 @@
       <c r="M42" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="N42" s="85"/>
-      <c r="O42" s="85"/>
+      <c r="N42" s="58"/>
+      <c r="O42" s="58"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -4651,7 +4320,7 @@
         <v>5557826541</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>122</v>
@@ -4659,8 +4328,8 @@
       <c r="M43" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="N43" s="85"/>
-      <c r="O43" s="85"/>
+      <c r="N43" s="58"/>
+      <c r="O43" s="58"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
@@ -4694,7 +4363,7 @@
         <v>5554237891</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>122</v>
@@ -4702,18 +4371,18 @@
       <c r="M44" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="N44" s="85"/>
-      <c r="O44" s="85"/>
+      <c r="N44" s="58"/>
+      <c r="O44" s="58"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>47</v>
@@ -4722,7 +4391,7 @@
         <v>34108</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>131</v>
@@ -4744,17 +4413,17 @@
         <v>122</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="N45" s="85"/>
-      <c r="O45" s="85"/>
+        <v>289</v>
+      </c>
+      <c r="N45" s="58"/>
+      <c r="O45" s="58"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>186</v>
@@ -4781,7 +4450,7 @@
         <v>90165328917</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>122</v>
@@ -4789,8 +4458,8 @@
       <c r="M46" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N46" s="85"/>
-      <c r="O46" s="85"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="58"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
@@ -4830,8 +4499,8 @@
       <c r="M47" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N47" s="85"/>
-      <c r="O47" s="85"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
@@ -4873,8 +4542,8 @@
       <c r="M48" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N48" s="85"/>
-      <c r="O48" s="85"/>
+      <c r="N48" s="58"/>
+      <c r="O48" s="58"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
@@ -4916,8 +4585,8 @@
       <c r="M49" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N49" s="85"/>
-      <c r="O49" s="85"/>
+      <c r="N49" s="58"/>
+      <c r="O49" s="58"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
@@ -4959,8 +4628,8 @@
       <c r="M50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N50" s="85"/>
-      <c r="O50" s="85"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="58"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
@@ -4980,10 +4649,10 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="N51" s="85"/>
-      <c r="O51" s="85"/>
+        <v>290</v>
+      </c>
+      <c r="N51" s="58"/>
+      <c r="O51" s="58"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J52" s="14"/>
@@ -5058,16 +4727,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -5093,14 +4763,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C2" s="56"/>
       <c r="D2" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E2" s="83" t="s">
-        <v>311</v>
+        <v>300</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5108,14 +4778,12 @@
         <v>2</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="56" t="s">
-        <v>310</v>
-      </c>
+      <c r="C3" s="56"/>
       <c r="D3" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>304</v>
+        <v>300</v>
+      </c>
+      <c r="E3" s="67" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -5125,10 +4793,10 @@
       <c r="B4" s="1"/>
       <c r="C4" s="56"/>
       <c r="D4" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>304</v>
+        <v>300</v>
+      </c>
+      <c r="E4" s="68" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5136,249 +4804,303 @@
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="56"/>
+      <c r="C5" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E5" s="59" t="s">
-        <v>305</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E5" s="58"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="56"/>
+      <c r="C6" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E6" s="60" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E6" s="58"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="56"/>
+      <c r="C7" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E7" s="61" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E7" s="58"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="56"/>
+      <c r="C8" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E8" s="58"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="56"/>
+      <c r="C9" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D9" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E9" s="63" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E9" s="58"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="56"/>
+      <c r="C10" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E10" s="64" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E10" s="58"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="56"/>
+      <c r="C11" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D11" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E11" s="65" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E11" s="58"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="56"/>
+      <c r="C12" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E12" s="66" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E12" s="58"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="56"/>
+      <c r="C13" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D13" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E13" s="67" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E13" s="58"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="56"/>
+      <c r="C14" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E14" s="68" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E14" s="58"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="56"/>
+      <c r="C15" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E15" s="69" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E15" s="58"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="56"/>
+      <c r="C16" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E16" s="70" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E16" s="58"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="56"/>
+      <c r="C17" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D17" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E17" s="71" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E17" s="58"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="56"/>
+      <c r="C18" s="56" t="s">
+        <v>284</v>
+      </c>
       <c r="D18" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E18" s="72" t="s">
-        <v>304</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="E18" s="58"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>304</v>
+      </c>
       <c r="C19" s="56"/>
       <c r="D19" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E19" s="73" t="s">
-        <v>304</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="E19" s="58"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1" t="s">
+        <v>306</v>
+      </c>
       <c r="C20" s="56"/>
       <c r="D20" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E20" s="74" t="s">
-        <v>304</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="E20" s="58"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="75">
+      <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="75" t="s">
-        <v>301</v>
-      </c>
-      <c r="E21" s="78" t="s">
-        <v>304</v>
-      </c>
+      <c r="B21" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="58"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="56"/>
+      <c r="B22" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C22" s="56" t="s">
+        <v>313</v>
+      </c>
       <c r="D22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="58"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="57">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C23" s="1">
+        <v>93069</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E22" s="79" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="77">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E23" s="80" t="s">
-        <v>308</v>
-      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1000201</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="57">
+        <v>24</v>
+      </c>
+      <c r="B25" s="61" t="s">
+        <v>311</v>
+      </c>
+      <c r="C25" s="1">
+        <v>10003459012</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="60"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="59"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="60"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5391,7 +5113,7 @@
   <dimension ref="B3:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5449,7 +5171,7 @@
         <v>52092</v>
       </c>
       <c r="I12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -5457,7 +5179,7 @@
         <v>6680</v>
       </c>
       <c r="I13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -5465,13 +5187,16 @@
         <v>91806</v>
       </c>
       <c r="I14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="35">
         <v>6453</v>
       </c>
+      <c r="I15" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="36">
@@ -5525,92 +5250,92 @@
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="39" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="40" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="41" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="44" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="45" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="46" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="47" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="48" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="50" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="51" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="54" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="55" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EditCustInfo added and changes completed for deleteCustInfo
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="336">
   <si>
     <t>testcaseID</t>
   </si>
@@ -670,9 +670,6 @@
     <t>pre@test.com</t>
   </si>
   <si>
-    <t>jos@test.com</t>
-  </si>
-  <si>
     <t>moh@test.com</t>
   </si>
   <si>
@@ -970,19 +967,73 @@
     <t>$%*(^%$</t>
   </si>
   <si>
-    <t>Pass - Customer Registered Successfully!!!</t>
-  </si>
-  <si>
-    <t>94493</t>
-  </si>
-  <si>
-    <t>45887</t>
-  </si>
-  <si>
-    <t>56120</t>
-  </si>
-  <si>
-    <t>Pass - Customer deleted Successfully</t>
+    <t xml:space="preserve">                  </t>
+  </si>
+  <si>
+    <t>Your User id is wrong please provide correct userid</t>
+  </si>
+  <si>
+    <t>Change in address</t>
+  </si>
+  <si>
+    <t>Change in city</t>
+  </si>
+  <si>
+    <t>Change in state</t>
+  </si>
+  <si>
+    <t>Change in pin</t>
+  </si>
+  <si>
+    <t>Change in mobile number</t>
+  </si>
+  <si>
+    <t>Change in email id</t>
+  </si>
+  <si>
+    <t>All fields changed to blank</t>
+  </si>
+  <si>
+    <t>Deleted customer</t>
+  </si>
+  <si>
+    <t>78 8th main CD road</t>
+  </si>
+  <si>
+    <t>20 5th main KT layout</t>
+  </si>
+  <si>
+    <t>21 5th main KT layout</t>
+  </si>
+  <si>
+    <t>22 5th main KT layout</t>
+  </si>
+  <si>
+    <t>josh123@test.com</t>
+  </si>
+  <si>
+    <t>Bidar</t>
+  </si>
+  <si>
+    <t>^*#%&amp;</t>
+  </si>
+  <si>
+    <t>When screen is not active</t>
+  </si>
+  <si>
+    <t>No Changes made to Customer records</t>
+  </si>
+  <si>
+    <t>No changes made to the customer id</t>
+  </si>
+  <si>
+    <t>Customer details updated Successfully!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               </t>
+  </si>
+  <si>
+    <t>jos@guest.com</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1064,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1077,38 +1128,8 @@
         <fgColor indexed="57"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="57"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="54">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -1815,102 +1836,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1976,12 +1907,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2469,8 +2394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:O4"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2563,7 +2488,7 @@
         <v>7771232345</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>214</v>
+        <v>335</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>122</v>
@@ -2571,12 +2496,8 @@
       <c r="M2" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="63" t="s">
-        <v>315</v>
-      </c>
-      <c r="O2" s="63" t="s">
-        <v>314</v>
-      </c>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -2610,7 +2531,7 @@
         <v>7778907689</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>122</v>
@@ -2618,12 +2539,8 @@
       <c r="M3" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N3" s="64" t="s">
-        <v>316</v>
-      </c>
-      <c r="O3" s="64" t="s">
-        <v>314</v>
-      </c>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -2657,7 +2574,7 @@
         <v>7771237890</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>122</v>
@@ -2665,12 +2582,8 @@
       <c r="M4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N4" s="65" t="s">
-        <v>317</v>
-      </c>
-      <c r="O4" s="65" t="s">
-        <v>314</v>
-      </c>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -2915,7 +2828,7 @@
         <v>7779081234</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>122</v>
@@ -2956,7 +2869,7 @@
         <v>7776892313</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>122</v>
@@ -3040,7 +2953,7 @@
         <v>2227657890</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>122</v>
@@ -3083,7 +2996,7 @@
         <v>90167189172</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>122</v>
@@ -3169,7 +3082,7 @@
         <v>4417678901</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>122</v>
@@ -3212,7 +3125,7 @@
         <v>4417657812</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>122</v>
@@ -3240,7 +3153,7 @@
         <v>34169</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="15" t="s">
@@ -3253,7 +3166,7 @@
         <v>9997863271</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>122</v>
@@ -3281,13 +3194,13 @@
         <v>33667</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I19" s="1">
         <v>879656</v>
@@ -3324,7 +3237,7 @@
         <v>32238</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G20" s="1">
         <v>56687</v>
@@ -3367,10 +3280,10 @@
         <v>33773</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>50</v>
@@ -3410,10 +3323,10 @@
         <v>33437</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>104</v>
@@ -3453,10 +3366,10 @@
         <v>35859</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1">
@@ -3494,13 +3407,13 @@
         <v>34158</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I24" s="1">
         <v>775645</v>
@@ -3537,10 +3450,10 @@
         <v>34432</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H25" s="1">
         <v>13345</v>
@@ -3580,13 +3493,13 @@
         <v>35163</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I26" s="1">
         <v>765435</v>
@@ -3623,13 +3536,13 @@
         <v>32971</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I27" s="1">
         <v>767546</v>
@@ -3666,10 +3579,10 @@
         <v>32975</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>156</v>
@@ -3707,16 +3620,16 @@
         <v>33733</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="I29" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J29" s="1">
         <v>5657811232</v>
@@ -3750,16 +3663,16 @@
         <v>34095</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>236</v>
-      </c>
       <c r="I30" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J30" s="1">
         <v>6628725671</v>
@@ -3793,16 +3706,16 @@
         <v>34888</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J31" s="1">
         <v>5529874561</v>
@@ -3836,13 +3749,13 @@
         <v>36025</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I32" s="1">
         <v>5654325</v>
@@ -3851,7 +3764,7 @@
         <v>5658901234</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>122</v>
@@ -3879,13 +3792,13 @@
         <v>34128</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="H33" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="I33" s="1">
         <v>5664</v>
@@ -3922,10 +3835,10 @@
         <v>34523</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>50</v>
@@ -3963,7 +3876,7 @@
         <v>35162</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>49</v>
@@ -4006,7 +3919,7 @@
         <v>35977</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>54</v>
@@ -4018,7 +3931,7 @@
         <v>778654</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>208</v>
@@ -4049,22 +3962,22 @@
         <v>34351</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="I37" s="1">
         <v>326787</v>
       </c>
       <c r="J37" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>122</v>
@@ -4092,13 +4005,13 @@
         <v>35527</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G38" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="I38" s="1">
         <v>456367</v>
@@ -4135,10 +4048,10 @@
         <v>34127</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>132</v>
@@ -4178,7 +4091,7 @@
         <v>34523</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>131</v>
@@ -4219,7 +4132,7 @@
         <v>35965</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>155</v>
@@ -4234,7 +4147,7 @@
         <v>4415427819</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>122</v>
@@ -4262,7 +4175,7 @@
         <v>34432</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>159</v>
@@ -4277,7 +4190,7 @@
         <v>4412568916</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>122</v>
@@ -4305,7 +4218,7 @@
         <v>32966</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>103</v>
@@ -4320,7 +4233,7 @@
         <v>5557826541</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>122</v>
@@ -4348,10 +4261,10 @@
         <v>33333</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>104</v>
@@ -4363,7 +4276,7 @@
         <v>5554237891</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>122</v>
@@ -4379,10 +4292,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>47</v>
@@ -4391,7 +4304,7 @@
         <v>34108</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>131</v>
@@ -4407,13 +4320,13 @@
       </c>
       <c r="K45" s="2" t="str">
         <f>K2</f>
-        <v>jos@test.com</v>
+        <v>jos@guest.com</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>122</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N45" s="58"/>
       <c r="O45" s="58"/>
@@ -4423,7 +4336,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>186</v>
@@ -4435,7 +4348,7 @@
         <v>33376</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>147</v>
@@ -4450,7 +4363,7 @@
         <v>90165328917</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>122</v>
@@ -4478,7 +4391,7 @@
         <v>35167</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>150</v>
@@ -4519,7 +4432,7 @@
         <v>34096</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>52</v>
@@ -4562,7 +4475,7 @@
         <v>33708</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>98</v>
@@ -4608,7 +4521,7 @@
         <v>144</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>132</v>
@@ -4620,7 +4533,7 @@
         <v>2226189271</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>192</v>
@@ -4649,7 +4562,7 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N51" s="58"/>
       <c r="O51" s="58"/>
@@ -4715,13 +4628,451 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1">
+        <v>566721</v>
+      </c>
+      <c r="H2" s="1">
+        <v>7771232345</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K2" s="58"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="1">
+        <v>566721</v>
+      </c>
+      <c r="H3" s="1">
+        <v>7771232345</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K3" s="58"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G4" s="1">
+        <v>566721</v>
+      </c>
+      <c r="H4" s="1">
+        <v>7771232345</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K4" s="58"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="1">
+        <v>543789</v>
+      </c>
+      <c r="H5" s="1">
+        <v>7771232345</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K5" s="58"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1">
+        <v>566721</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7778901237</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K6" s="58"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1">
+        <v>566721</v>
+      </c>
+      <c r="H7" s="1">
+        <v>7771232345</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K7" s="58"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="1">
+        <v>566721</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7771232345</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="K8" s="58"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="K9" s="58"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="K10" s="58"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K11" s="58"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K12" s="58"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K13" s="58"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C14" s="1">
+        <v>93069</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="K14" s="58"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12334</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="K15" s="58"/>
+    </row>
+    <row r="16" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="61" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1238905672</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="K16" s="58"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I6" r:id="rId5"/>
+    <hyperlink ref="I7" r:id="rId6"/>
+    <hyperlink ref="I8" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -4730,7 +5081,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4763,52 +5114,50 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C2" s="56"/>
       <c r="D2" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E2" s="66" t="s">
-        <v>318</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="E2" s="58"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>301</v>
+      </c>
       <c r="C3" s="56"/>
       <c r="D3" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E3" s="67" t="s">
-        <v>318</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="E3" s="58"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>301</v>
+      </c>
       <c r="C4" s="56"/>
       <c r="D4" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="E4" s="68" t="s">
-        <v>318</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="E4" s="58"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C5" s="56"/>
       <c r="D5" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E5" s="58"/>
     </row>
@@ -4816,12 +5165,12 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B6" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C6" s="56"/>
       <c r="D6" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E6" s="58"/>
     </row>
@@ -4829,12 +5178,12 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C7" s="56"/>
       <c r="D7" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E7" s="58"/>
     </row>
@@ -4842,12 +5191,12 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B8" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="56"/>
       <c r="D8" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E8" s="58"/>
     </row>
@@ -4855,12 +5204,12 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B9" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C9" s="56"/>
       <c r="D9" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E9" s="58"/>
     </row>
@@ -4868,12 +5217,12 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B10" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C10" s="56"/>
       <c r="D10" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E10" s="58"/>
     </row>
@@ -4881,12 +5230,12 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B11" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C11" s="56"/>
       <c r="D11" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E11" s="58"/>
     </row>
@@ -4894,12 +5243,12 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B12" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C12" s="56"/>
       <c r="D12" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E12" s="58"/>
     </row>
@@ -4907,12 +5256,12 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B13" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C13" s="56"/>
       <c r="D13" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E13" s="58"/>
     </row>
@@ -4920,12 +5269,12 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B14" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C14" s="56"/>
       <c r="D14" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E14" s="58"/>
     </row>
@@ -4933,12 +5282,12 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B15" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C15" s="56"/>
       <c r="D15" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E15" s="58"/>
     </row>
@@ -4946,12 +5295,12 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B16" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C16" s="56"/>
       <c r="D16" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E16" s="58"/>
     </row>
@@ -4959,12 +5308,12 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B17" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C17" s="56"/>
       <c r="D17" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E17" s="58"/>
     </row>
@@ -4972,12 +5321,12 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="56" t="s">
-        <v>284</v>
-      </c>
+      <c r="B18" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C18" s="56"/>
       <c r="D18" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E18" s="58"/>
     </row>
@@ -4986,11 +5335,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E19" s="58"/>
     </row>
@@ -4999,9 +5348,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C20" s="56"/>
+        <v>305</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>313</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>126</v>
       </c>
@@ -5012,10 +5363,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C21" s="56" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>138</v>
@@ -5027,10 +5378,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>128</v>
@@ -5042,45 +5393,45 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C23" s="1">
         <v>93069</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>300</v>
+      </c>
+      <c r="E23" s="58"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C24" s="1">
         <v>1000201</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>300</v>
+      </c>
+      <c r="E24" s="58"/>
     </row>
     <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="57">
         <v>24</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C25" s="1">
         <v>10003459012</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>300</v>
+      </c>
+      <c r="E25" s="58"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="59"/>
@@ -5110,95 +5461,102 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I51"/>
+  <dimension ref="B3:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="9.140625" style="31" collapsed="1"/>
+    <col min="9" max="9" width="46.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="17">
         <v>43455</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="18">
         <v>39551</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="19">
         <v>25023</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>99287</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="19">
         <v>44146</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="19">
         <v>55287</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="32">
         <v>6671</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="20">
         <v>88191</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="21">
         <v>98587</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="33">
         <v>52092</v>
       </c>
       <c r="I12" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="22">
         <v>6680</v>
       </c>
       <c r="I13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="34">
         <v>91806</v>
       </c>
       <c r="I14" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="35">
         <v>6453</v>
       </c>
       <c r="I15" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="J15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="36">
         <v>83119</v>
       </c>
@@ -5250,92 +5608,92 @@
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="39" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="41" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="44" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="45" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="46" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="47" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="48" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="49" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="50" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="51" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="53" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="54" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="55" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new account and delete new account changes WIP Edit account skeleton added
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
@@ -4,17 +4,27 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="NewCust" sheetId="2" r:id="rId2"/>
-    <sheet name="EditCust" sheetId="3" r:id="rId3"/>
-    <sheet name="DeleteCust" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId2"/>
+    <sheet name="NewCust" sheetId="2" r:id="rId3"/>
+    <sheet name="EditCust" sheetId="3" r:id="rId4"/>
+    <sheet name="DeleteCust" sheetId="7" r:id="rId5"/>
+    <sheet name="NewAcct" sheetId="8" r:id="rId6"/>
+    <sheet name="EditAcct" sheetId="9" r:id="rId7"/>
+    <sheet name="DeleteAcct" sheetId="10" r:id="rId8"/>
+    <sheet name="Deposit" sheetId="11" r:id="rId9"/>
+    <sheet name="Withdrawal" sheetId="12" r:id="rId10"/>
+    <sheet name="Fund Transfer" sheetId="13" r:id="rId11"/>
+    <sheet name="BalEnquiry" sheetId="14" r:id="rId12"/>
+    <sheet name="MiniStat" sheetId="15" r:id="rId13"/>
+    <sheet name="CustStat" sheetId="16" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">NewCust!$M$1:$M$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">NewAcct!$F$1:$F$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewCust!$M$1:$M$52</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="391">
   <si>
     <t>testcaseID</t>
   </si>
@@ -877,170 +887,335 @@
     <t>keit@test.com</t>
   </si>
   <si>
+    <t>Existing email id</t>
+  </si>
+  <si>
+    <t>Jilka</t>
+  </si>
+  <si>
+    <t>544 8th main GKV road</t>
+  </si>
+  <si>
+    <t>sanya@test.com</t>
+  </si>
+  <si>
+    <t>Email Address Already Exist !!</t>
+  </si>
+  <si>
+    <t>Customer name must not be blankDate Field must not be blankAddress Field must not be blankCity Field must not be blankState must not be blankPIN Code must not be blankMobile no must not be blankEmail-ID must not be blankPassword must not be blank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 </t>
+  </si>
+  <si>
+    <t>rootest.com</t>
+  </si>
+  <si>
+    <t>vee@test</t>
+  </si>
+  <si>
+    <t>dar</t>
+  </si>
+  <si>
+    <t>^&amp;*%%&amp;*</t>
+  </si>
+  <si>
+    <t>kiran@test.com</t>
+  </si>
+  <si>
+    <t>Email id exceeding 30 characters</t>
+  </si>
+  <si>
+    <t>ali12345678901234562@test.com11</t>
+  </si>
+  <si>
+    <t>Customer deleted Successfully</t>
+  </si>
+  <si>
+    <t>Customer does not exist!!</t>
+  </si>
+  <si>
+    <t>Existing customer id</t>
+  </si>
+  <si>
+    <t>Customer ID is required</t>
+  </si>
+  <si>
+    <t>Blank customer id</t>
+  </si>
+  <si>
+    <t>You are not authorize to delete this customer!!</t>
+  </si>
+  <si>
+    <t>Only spaces in customer id</t>
+  </si>
+  <si>
+    <t>Characters in customer id</t>
+  </si>
+  <si>
+    <t>Special characters in customer id</t>
+  </si>
+  <si>
+    <t>Non existing customer id</t>
+  </si>
+  <si>
+    <t>Previously deleted customer id</t>
+  </si>
+  <si>
+    <t>Customer id exceeding 10 digits(Generated ids are &lt;10 digits as of now, hence non existing 11 digits customer id is used for testing)</t>
+  </si>
+  <si>
+    <t>customerid</t>
+  </si>
+  <si>
+    <t>$%*(^%$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  </t>
+  </si>
+  <si>
+    <t>Your User id is wrong please provide correct userid</t>
+  </si>
+  <si>
+    <t>Change in address</t>
+  </si>
+  <si>
+    <t>Change in city</t>
+  </si>
+  <si>
+    <t>Change in state</t>
+  </si>
+  <si>
+    <t>Change in pin</t>
+  </si>
+  <si>
+    <t>Change in mobile number</t>
+  </si>
+  <si>
+    <t>Change in email id</t>
+  </si>
+  <si>
+    <t>All fields changed to blank</t>
+  </si>
+  <si>
+    <t>Deleted customer</t>
+  </si>
+  <si>
+    <t>78 8th main CD road</t>
+  </si>
+  <si>
+    <t>20 5th main KT layout</t>
+  </si>
+  <si>
+    <t>21 5th main KT layout</t>
+  </si>
+  <si>
+    <t>22 5th main KT layout</t>
+  </si>
+  <si>
+    <t>josh123@test.com</t>
+  </si>
+  <si>
+    <t>Bidar</t>
+  </si>
+  <si>
+    <t>^*#%&amp;</t>
+  </si>
+  <si>
+    <t>No Changes made to Customer records</t>
+  </si>
+  <si>
+    <t>No changes made to the customer id</t>
+  </si>
+  <si>
+    <t>Customer details updated Successfully!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               </t>
+  </si>
+  <si>
+    <t>jos@guest.com</t>
+  </si>
+  <si>
+    <t>http://demo.guru99.com/v4/manager/Managerhomepage.php</t>
+  </si>
+  <si>
+    <t>You are not authorize to edit this customer!!</t>
+  </si>
+  <si>
+    <t>Open the link w/o credential and perform add new cust</t>
+  </si>
+  <si>
+    <t>open the link w/o credential and perform edit cust</t>
+  </si>
+  <si>
+    <t>open the link w/o credential and perform delete cust</t>
+  </si>
+  <si>
+    <t>Custid</t>
+  </si>
+  <si>
+    <t>Accountid</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Guru@2018</t>
+  </si>
+  <si>
+    <t>AcctType</t>
+  </si>
+  <si>
+    <t>One account with multiple saving accounts</t>
+  </si>
+  <si>
+    <t>One account with multiple current accounts</t>
+  </si>
+  <si>
+    <t>Customer could not be deleted!!. First delete all accounts of this customer then delete the customer</t>
+  </si>
+  <si>
+    <t>Trying to delete a customer with account tagged customer id</t>
+  </si>
+  <si>
+    <t>Add a new  savings account</t>
+  </si>
+  <si>
+    <t>Add a new current account</t>
+  </si>
+  <si>
+    <t>Add a new savings account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special characters in customer </t>
+  </si>
+  <si>
+    <t>Non-existing customer id</t>
+  </si>
+  <si>
+    <t>Blank initial deposit</t>
+  </si>
+  <si>
+    <t>Only spaces in initial deposit</t>
+  </si>
+  <si>
+    <t>Characters in initial deposit</t>
+  </si>
+  <si>
+    <t>Special characters in initial deposit</t>
+  </si>
+  <si>
+    <t>Initial deposit less than 500</t>
+  </si>
+  <si>
+    <t>Initial deposit of 500</t>
+  </si>
+  <si>
+    <t>Initial deposit greater than 500</t>
+  </si>
+  <si>
+    <t>Initial deposit exceeding 8 digits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              </t>
+  </si>
+  <si>
+    <t>$&amp;^%#</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>deposit</t>
+  </si>
+  <si>
+    <t>$#&amp;*)(</t>
+  </si>
+  <si>
+    <t>InitialDeposit</t>
+  </si>
+  <si>
+    <t>Account Generated Successfully!!!</t>
+  </si>
+  <si>
+    <t>Initial Deposit must not be blank</t>
+  </si>
+  <si>
+    <t>Intial deposite must be Rs. 500 or more</t>
+  </si>
+  <si>
+    <t>Customer ID is requiredInitial Deposit must not be blank</t>
+  </si>
+  <si>
+    <t>Blank Account type</t>
+  </si>
+  <si>
+    <t>Existing account number</t>
+  </si>
+  <si>
+    <t>acctnum</t>
+  </si>
+  <si>
+    <t>Deleting a customer id with active accounts</t>
+  </si>
+  <si>
+    <t>Blank account number</t>
+  </si>
+  <si>
+    <t>Account Number must not be blank</t>
+  </si>
+  <si>
+    <t>Only spaces in account number</t>
+  </si>
+  <si>
+    <t>Characters in account number</t>
+  </si>
+  <si>
+    <t>Special characters in account number</t>
+  </si>
+  <si>
+    <t>Previously deleted account number</t>
+  </si>
+  <si>
+    <t>Non existing account number</t>
+  </si>
+  <si>
+    <t>Account number exceeding 10 digits(Generated numbers are &lt;10 digits as of now, hence non existing 11 digits account number is used for testing)</t>
+  </si>
+  <si>
+    <t>accountno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     </t>
+  </si>
+  <si>
+    <t>Account does not exist</t>
+  </si>
+  <si>
+    <t>Account Deleted Sucessfully</t>
+  </si>
+  <si>
+    <t>Pass - Account Generated Successfully!!!</t>
+  </si>
+  <si>
+    <t>39283</t>
+  </si>
+  <si>
+    <t>Pass - Account Deleted Sucessfully</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>Existing email id</t>
-  </si>
-  <si>
-    <t>Jilka</t>
-  </si>
-  <si>
-    <t>544 8th main GKV road</t>
-  </si>
-  <si>
-    <t>sanya@test.com</t>
-  </si>
-  <si>
-    <t>Email Address Already Exist !!</t>
-  </si>
-  <si>
-    <t>Customer name must not be blankDate Field must not be blankAddress Field must not be blankCity Field must not be blankState must not be blankPIN Code must not be blankMobile no must not be blankEmail-ID must not be blankPassword must not be blank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                 </t>
-  </si>
-  <si>
-    <t>rootest.com</t>
-  </si>
-  <si>
-    <t>vee@test</t>
-  </si>
-  <si>
-    <t>dar</t>
-  </si>
-  <si>
-    <t>^&amp;*%%&amp;*</t>
-  </si>
-  <si>
-    <t>kiran@test.com</t>
-  </si>
-  <si>
-    <t>Email id exceeding 30 characters</t>
-  </si>
-  <si>
-    <t>ali12345678901234562@test.com11</t>
-  </si>
-  <si>
-    <t>Do you really want to delete this Customer?</t>
-  </si>
-  <si>
-    <t>Customer deleted Successfully</t>
-  </si>
-  <si>
-    <t>Customer does not exist!!</t>
-  </si>
-  <si>
-    <t>Existing customer id</t>
-  </si>
-  <si>
-    <t>Customer ID is required</t>
-  </si>
-  <si>
-    <t>Blank customer id</t>
-  </si>
-  <si>
-    <t>You are not authorize to delete this customer!!</t>
-  </si>
-  <si>
-    <t>Only spaces in customer id</t>
-  </si>
-  <si>
-    <t>Characters in customer id</t>
-  </si>
-  <si>
-    <t>Special characters in customer id</t>
-  </si>
-  <si>
-    <t>Non existing customer id</t>
-  </si>
-  <si>
-    <t>Previously deleted customer id</t>
-  </si>
-  <si>
-    <t>Customer id exceeding 10 digits(Generated ids are &lt;10 digits as of now, hence non existing 11 digits customer id is used for testing)</t>
-  </si>
-  <si>
-    <t>customerid</t>
-  </si>
-  <si>
-    <t>$%*(^%$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  </t>
-  </si>
-  <si>
-    <t>Your User id is wrong please provide correct userid</t>
-  </si>
-  <si>
-    <t>Change in address</t>
-  </si>
-  <si>
-    <t>Change in city</t>
-  </si>
-  <si>
-    <t>Change in state</t>
-  </si>
-  <si>
-    <t>Change in pin</t>
-  </si>
-  <si>
-    <t>Change in mobile number</t>
-  </si>
-  <si>
-    <t>Change in email id</t>
-  </si>
-  <si>
-    <t>All fields changed to blank</t>
-  </si>
-  <si>
-    <t>Deleted customer</t>
-  </si>
-  <si>
-    <t>78 8th main CD road</t>
-  </si>
-  <si>
-    <t>20 5th main KT layout</t>
-  </si>
-  <si>
-    <t>21 5th main KT layout</t>
-  </si>
-  <si>
-    <t>22 5th main KT layout</t>
-  </si>
-  <si>
-    <t>josh123@test.com</t>
-  </si>
-  <si>
-    <t>Bidar</t>
-  </si>
-  <si>
-    <t>^*#%&amp;</t>
-  </si>
-  <si>
-    <t>When screen is not active</t>
-  </si>
-  <si>
-    <t>No Changes made to Customer records</t>
-  </si>
-  <si>
-    <t>No changes made to the customer id</t>
-  </si>
-  <si>
-    <t>Customer details updated Successfully!!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               </t>
-  </si>
-  <si>
-    <t>jos@guest.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1063,8 +1238,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1124,12 +1322,44 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="solid">
         <fgColor indexed="57"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1836,12 +2066,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1906,7 +2181,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="47" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2188,10 +2486,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="E9" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="37.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.140625" style="31" collapsed="1"/>
+    <col min="8" max="8" width="58" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="46.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="18"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
+      <c r="H7" s="73" t="s">
+        <v>333</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="64" t="s">
+        <v>346</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="21"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="33"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="34"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+    </row>
+    <row r="16" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="36"/>
+      <c r="H16" s="66" t="s">
+        <v>338</v>
+      </c>
+      <c r="I16" s="66" t="s">
+        <v>339</v>
+      </c>
+      <c r="J16" s="67" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="37"/>
+      <c r="H17" s="75">
+        <v>2102</v>
+      </c>
+      <c r="I17" s="65">
+        <v>39256</v>
+      </c>
+      <c r="J17" s="65">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="68"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="65">
+        <v>39275</v>
+      </c>
+      <c r="J18" s="65">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="68"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="65">
+        <v>39280</v>
+      </c>
+      <c r="J19" s="65">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="68"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="65">
+        <v>39281</v>
+      </c>
+      <c r="J20" s="65">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="23"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="65">
+        <v>39279</v>
+      </c>
+      <c r="J21" s="65">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="24"/>
+      <c r="H22" s="74">
+        <v>94925</v>
+      </c>
+      <c r="I22" s="65">
+        <v>39276</v>
+      </c>
+      <c r="J22" s="65">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="25"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="65">
+        <v>39277</v>
+      </c>
+      <c r="J23" s="65">
+        <v>5001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="26"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="65">
+        <v>39278</v>
+      </c>
+      <c r="J24" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="27"/>
+      <c r="H25" s="74">
+        <v>89280</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="28"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="29"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="30"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="38"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="39"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="40"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="41"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="42"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="43"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="44"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="45"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="46"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="47"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="48"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="49"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="50"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="51"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="52"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="53"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="54"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="H25:H27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,6 +2842,7 @@
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="51.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="55.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -2239,13 +2883,13 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
+      <c r="E2" s="2" t="s">
+        <v>341</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="71" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2384,18 +3028,19 @@
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3:C5" r:id="rId2" display="http://demo.guru99.com/v4/"/>
     <hyperlink ref="C6:C8" r:id="rId3" display="http://demo.guru99.com/v4/"/>
+    <hyperlink ref="E2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,7 +3133,7 @@
         <v>7771232345</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>122</v>
@@ -3764,7 +4409,7 @@
         <v>5658901234</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>122</v>
@@ -3974,10 +4619,10 @@
         <v>326787</v>
       </c>
       <c r="J37" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>122</v>
@@ -4147,7 +4792,7 @@
         <v>4415427819</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>122</v>
@@ -4190,7 +4835,7 @@
         <v>4412568916</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>122</v>
@@ -4233,7 +4878,7 @@
         <v>5557826541</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>122</v>
@@ -4276,7 +4921,7 @@
         <v>5554237891</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>122</v>
@@ -4292,10 +4937,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>284</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>285</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>47</v>
@@ -4304,7 +4949,7 @@
         <v>34108</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>131</v>
@@ -4326,7 +4971,7 @@
         <v>122</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N45" s="58"/>
       <c r="O45" s="58"/>
@@ -4336,7 +4981,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>186</v>
@@ -4363,7 +5008,7 @@
         <v>90165328917</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>122</v>
@@ -4562,13 +5207,16 @@
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N51" s="58"/>
       <c r="O51" s="58"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J52" s="14"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="62"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4620,18 +5268,19 @@
     <hyperlink ref="K49" r:id="rId46"/>
     <hyperlink ref="K50" r:id="rId47"/>
     <hyperlink ref="K45" r:id="rId48" display="kei@test.com"/>
+    <hyperlink ref="K12" r:id="rId49" display="simran@test.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId49"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4685,11 +5334,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>49</v>
@@ -4704,10 +5353,10 @@
         <v>7771232345</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K2" s="58"/>
     </row>
@@ -4716,14 +5365,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>50</v>
@@ -4735,10 +5384,10 @@
         <v>7771232345</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K3" s="58"/>
     </row>
@@ -4747,7 +5396,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
@@ -4766,10 +5415,10 @@
         <v>7771232345</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K4" s="58"/>
     </row>
@@ -4778,11 +5427,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>49</v>
@@ -4797,10 +5446,10 @@
         <v>7771232345</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K5" s="58"/>
     </row>
@@ -4809,11 +5458,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>49</v>
@@ -4828,10 +5477,10 @@
         <v>7778901237</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K6" s="58"/>
     </row>
@@ -4840,11 +5489,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>49</v>
@@ -4859,10 +5508,10 @@
         <v>7771232345</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K7" s="58"/>
     </row>
@@ -4871,11 +5520,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>49</v>
@@ -4890,10 +5539,10 @@
         <v>7771232345</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="K8" s="58"/>
     </row>
@@ -4902,7 +5551,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -4912,7 +5561,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="2"/>
       <c r="J9" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K9" s="58"/>
     </row>
@@ -4921,7 +5570,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -4931,7 +5580,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K10" s="58"/>
     </row>
@@ -4940,10 +5589,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -4961,7 +5610,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
@@ -4982,10 +5631,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -5003,7 +5652,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C14" s="1">
         <v>93069</v>
@@ -5015,7 +5664,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K14" s="58"/>
     </row>
@@ -5024,7 +5673,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C15" s="1">
         <v>12334</v>
@@ -5036,7 +5685,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K15" s="58"/>
     </row>
@@ -5045,7 +5694,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="61" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C16" s="1">
         <v>1238905672</v>
@@ -5057,7 +5706,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K16" s="58"/>
     </row>
@@ -5076,12 +5725,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5114,11 +5763,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C2" s="56"/>
       <c r="D2" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E2" s="58"/>
     </row>
@@ -5127,11 +5776,11 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C3" s="56"/>
       <c r="D3" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E3" s="58"/>
     </row>
@@ -5140,11 +5789,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E4" s="58"/>
     </row>
@@ -5153,11 +5802,11 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E5" s="58"/>
     </row>
@@ -5166,11 +5815,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E6" s="58"/>
     </row>
@@ -5179,11 +5828,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E7" s="58"/>
     </row>
@@ -5192,11 +5841,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E8" s="58"/>
     </row>
@@ -5205,11 +5854,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C9" s="56"/>
       <c r="D9" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E9" s="58"/>
     </row>
@@ -5218,11 +5867,11 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C10" s="56"/>
       <c r="D10" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E10" s="58"/>
     </row>
@@ -5231,11 +5880,11 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C11" s="56"/>
       <c r="D11" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E11" s="58"/>
     </row>
@@ -5244,11 +5893,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C12" s="56"/>
       <c r="D12" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E12" s="58"/>
     </row>
@@ -5257,11 +5906,11 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E13" s="58"/>
     </row>
@@ -5270,11 +5919,11 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E14" s="58"/>
     </row>
@@ -5283,11 +5932,11 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E15" s="58"/>
     </row>
@@ -5296,11 +5945,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E16" s="58"/>
     </row>
@@ -5309,11 +5958,11 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E17" s="58"/>
     </row>
@@ -5322,11 +5971,11 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E18" s="58"/>
     </row>
@@ -5335,11 +5984,11 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E19" s="58"/>
     </row>
@@ -5348,10 +5997,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>126</v>
@@ -5363,10 +6012,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C21" s="56" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>138</v>
@@ -5378,10 +6027,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>128</v>
@@ -5393,13 +6042,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C23" s="1">
         <v>93069</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E23" s="58"/>
     </row>
@@ -5408,13 +6057,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C24" s="1">
         <v>1000201</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E24" s="58"/>
     </row>
@@ -5423,20 +6072,30 @@
         <v>24</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C25" s="1">
         <v>10003459012</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E25" s="58"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
+      <c r="A26" s="69">
+        <v>25</v>
+      </c>
+      <c r="B26" s="69" t="s">
+        <v>374</v>
+      </c>
+      <c r="C26" s="69">
+        <v>2102</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="60"/>
@@ -5459,244 +6118,958 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J51"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="9.140625" style="31" collapsed="1"/>
-    <col min="9" max="9" width="46.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="52" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="17">
-        <v>43455</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="18">
-        <v>39551</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="19">
-        <v>25023</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="19">
-        <v>99287</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="19">
-        <v>44146</v>
-      </c>
-      <c r="I7" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="19">
-        <v>55287</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="32">
-        <v>6671</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="20">
-        <v>88191</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="21">
-        <v>98587</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="33">
-        <v>52092</v>
-      </c>
-      <c r="I12" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2102</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>388</v>
+      </c>
+      <c r="H2" s="70" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2102</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" s="1">
+        <v>89280</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" s="1">
+        <v>89280</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4600</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2102</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1200</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2102</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1600</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1900</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1234</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="22">
-        <v>6680</v>
-      </c>
-      <c r="I13" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="34">
-        <v>91806</v>
-      </c>
-      <c r="I14" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="35">
-        <v>6453</v>
-      </c>
-      <c r="I15" t="s">
-        <v>304</v>
-      </c>
-      <c r="J15" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="36">
-        <v>83119</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="37">
-        <v>98074</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="23">
-        <v>69389</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="24">
-        <v>51934</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="25">
-        <v>35485</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="26">
-        <v>36131</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="27">
-        <v>25974</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="28">
-        <v>1839</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="29">
-        <v>86818</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="30">
-        <v>4904</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="38" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="39" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="40" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="41" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="42" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="44" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="45" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="47" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="48" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="49" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="50" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="51" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="52" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="53" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="54" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="55" t="s">
-        <v>283</v>
-      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2102</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>600</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C14" s="1">
+        <v>94925</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C15" s="1">
+        <v>94925</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C16" s="1">
+        <v>94925</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C17" s="1">
+        <v>94925</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C18" s="1">
+        <v>94925</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E18" s="1">
+        <v>499</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C19" s="1">
+        <v>94925</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E19" s="1">
+        <v>500</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C20" s="1">
+        <v>94925</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E20" s="1">
+        <v>501</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C21" s="1">
+        <v>94925</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E21" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C22" s="1">
+        <v>89280</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="E22" s="1">
+        <v>499</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C23" s="1">
+        <v>89280</v>
+      </c>
+      <c r="D23" s="64" t="s">
+        <v>363</v>
+      </c>
+      <c r="E23" s="1">
+        <v>500</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C24" s="1">
+        <v>89280</v>
+      </c>
+      <c r="D24" s="64" t="s">
+        <v>363</v>
+      </c>
+      <c r="E24" s="1">
+        <v>501</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C25" s="1">
+        <v>89280</v>
+      </c>
+      <c r="D25" s="64" t="s">
+        <v>363</v>
+      </c>
+      <c r="E25" s="1">
+        <v>200000000</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>390</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C3" s="56"/>
+      <c r="D3" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E3" s="58"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E4" s="58"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E5" s="58"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E6" s="58"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E7" s="58"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E8" s="58"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C9" s="56"/>
+      <c r="D9" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E9" s="58"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E10" s="58"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E11" s="58"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C12" s="56"/>
+      <c r="D12" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E12" s="58"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C13" s="56"/>
+      <c r="D13" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E13" s="58"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C14" s="56"/>
+      <c r="D14" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E14" s="58"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="C15" s="56"/>
+      <c r="D15" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E15" s="58"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>384</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="58"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>383</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="58"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>310</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="58"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C19" s="1">
+        <v>39282</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E19" s="58"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1239682</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E20" s="58"/>
+    </row>
+    <row r="21" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>382</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45003459012</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="E21" s="58"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes w.r.t balEnquiry and deposit
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="418">
   <si>
     <t>testcaseID</t>
   </si>
@@ -1212,6 +1212,84 @@
   </si>
   <si>
     <t>Write the latest balance to withdrawal to get the base</t>
+  </si>
+  <si>
+    <t>mngr124532</t>
+  </si>
+  <si>
+    <t>Existing savings account</t>
+  </si>
+  <si>
+    <t>Existing current account</t>
+  </si>
+  <si>
+    <t>Only Spaces in account number</t>
+  </si>
+  <si>
+    <t>Deleted account number</t>
+  </si>
+  <si>
+    <t>Account number exceeding 10 digits</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>#$%%^</t>
+  </si>
+  <si>
+    <t>Pass - Guru99 Bank Manager HomePage</t>
+  </si>
+  <si>
+    <t>Balance Details for Account</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>Pass - Account Number must not be blank</t>
+  </si>
+  <si>
+    <t>Pass - Characters are not allowed</t>
+  </si>
+  <si>
+    <t>Pass - Special characters are not allowed</t>
+  </si>
+  <si>
+    <t>Pass - Account does not exist</t>
+  </si>
+  <si>
+    <t>balBefore</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>currentbal</t>
+  </si>
+  <si>
+    <t>You are not authorize to deposit money in this account!!</t>
+  </si>
+  <si>
+    <t>fourth deposit</t>
+  </si>
+  <si>
+    <t>Transaction details of Deposit for Account</t>
+  </si>
+  <si>
+    <t>800</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1349,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1332,8 +1410,53 @@
         <fgColor indexed="57"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="43">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -1965,12 +2088,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2042,6 +2300,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2051,7 +2319,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2335,7 +2602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="E9" workbookViewId="0">
+    <sheetView topLeftCell="H13" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -2361,7 +2628,7 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
-      <c r="H7" s="65" t="s">
+      <c r="H7" s="75" t="s">
         <v>328</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -2373,7 +2640,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="H8" s="65"/>
+      <c r="H8" s="75"/>
       <c r="I8" s="1" t="s">
         <v>331</v>
       </c>
@@ -2383,7 +2650,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="25"/>
-      <c r="H9" s="65"/>
+      <c r="H9" s="75"/>
       <c r="I9" s="1" t="s">
         <v>332</v>
       </c>
@@ -2445,95 +2712,67 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="30"/>
-      <c r="H17" s="67">
-        <v>2102</v>
+      <c r="H17" s="77">
+        <v>37672</v>
       </c>
       <c r="I17" s="58">
-        <v>39275</v>
-      </c>
-      <c r="J17" s="58">
-        <v>5010</v>
-      </c>
+        <v>39905</v>
+      </c>
+      <c r="J17" s="58"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="61"/>
-      <c r="H18" s="67"/>
+      <c r="H18" s="77"/>
       <c r="I18" s="58">
-        <v>39280</v>
-      </c>
-      <c r="J18" s="58">
-        <v>3500</v>
-      </c>
+        <v>39906</v>
+      </c>
+      <c r="J18" s="58"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="61"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="58">
-        <v>39281</v>
-      </c>
-      <c r="J19" s="58">
-        <v>1000</v>
-      </c>
+      <c r="H19" s="77"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="61"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="58">
-        <v>39279</v>
-      </c>
-      <c r="J20" s="58">
-        <v>590</v>
-      </c>
+      <c r="H20" s="77"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
-      <c r="H21" s="66">
-        <v>94925</v>
-      </c>
-      <c r="I21" s="58">
-        <v>39276</v>
-      </c>
-      <c r="J21" s="58">
-        <v>500</v>
-      </c>
+      <c r="H21" s="76"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="58"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="18"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="58">
-        <v>39277</v>
-      </c>
-      <c r="J22" s="58">
-        <v>5001</v>
-      </c>
+      <c r="H22" s="76"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="19"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="58">
-        <v>39278</v>
-      </c>
-      <c r="J23" s="1">
-        <v>600</v>
-      </c>
+      <c r="H23" s="76"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="1"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="20"/>
-      <c r="H24" s="66">
-        <v>89280</v>
-      </c>
+      <c r="H24" s="76"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="21"/>
-      <c r="H25" s="66"/>
+      <c r="H25" s="76"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="22"/>
-      <c r="H26" s="66"/>
+      <c r="H26" s="76"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
@@ -2632,31 +2871,215 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="R13:R15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="13" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R13" s="68" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C2" s="1">
+        <v>39905</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E2" s="51" t="s">
+        <v>417</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="C3" s="1">
+        <v>39906</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="F3" s="67" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E4" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="F5" s="69" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F6" s="70" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="14" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R14" s="68" t="s">
+      <c r="E7" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F7" s="71" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C8" s="1">
+        <v>39276</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F8" s="72" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C9" s="1">
+        <v>34587690128</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F9" s="73" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S13" s="65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S14" s="65" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="18:18" x14ac:dyDescent="0.25">
-      <c r="R15" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
         <v>389</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2689,7 +3112,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,7 +3159,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>392</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>336</v>
@@ -2744,7 +3167,9 @@
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="51"/>
+      <c r="G2" s="74" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -6575,7 +7000,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6607,8 +7032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6616,7 +7041,7 @@
     <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6920,32 +7345,97 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:J12"/>
+  <dimension ref="H1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="38.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="1" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="J2" s="1">
+        <v>39905</v>
+      </c>
+      <c r="K2" s="1">
+        <v>800</v>
+      </c>
+      <c r="L2" s="1">
+        <v>250</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="23" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U23" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="24" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U24" s="65" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="26" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U26" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="27" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U27" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J11" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="J12" s="68" t="s">
-        <v>388</v>
+    <row r="28" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U28" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes related deposit and withdrawal completed
</commit_message>
<xml_diff>
--- a/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
+++ b/SeleniumWebDriver/src/guru99/DataFiles/Guru99_testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="NewAcct" sheetId="8" r:id="rId6"/>
     <sheet name="EditAcct" sheetId="9" r:id="rId7"/>
     <sheet name="DeleteAcct" sheetId="10" r:id="rId8"/>
-    <sheet name="Deposit" sheetId="11" r:id="rId9"/>
+    <sheet name="Deposit" sheetId="18" r:id="rId9"/>
     <sheet name="Withdrawal" sheetId="12" r:id="rId10"/>
     <sheet name="FundTransfer" sheetId="13" r:id="rId11"/>
     <sheet name="BalEnquiry" sheetId="17" r:id="rId12"/>
@@ -35,8 +35,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C18" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Need to create new accounts else balBefore would be wrong</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="450">
   <si>
     <t>testcaseID</t>
   </si>
@@ -1202,18 +1236,9 @@
     <t>You Have Succesfully Logged Out!!</t>
   </si>
   <si>
-    <t>Transaction details of Deposit for Account 39275</t>
-  </si>
-  <si>
     <t>pop-up &gt; Account does not exist</t>
   </si>
   <si>
-    <t>Get the balance from balEnquiry as one of the input here and add the amount to validate the latest balance after deposit</t>
-  </si>
-  <si>
-    <t>Write the latest balance to withdrawal to get the base</t>
-  </si>
-  <si>
     <t>mngr124532</t>
   </si>
   <si>
@@ -1283,20 +1308,125 @@
     <t>You are not authorize to deposit money in this account!!</t>
   </si>
   <si>
-    <t>fourth deposit</t>
-  </si>
-  <si>
     <t>Transaction details of Deposit for Account</t>
   </si>
   <si>
     <t>800</t>
+  </si>
+  <si>
+    <t>savings investment</t>
+  </si>
+  <si>
+    <t>current investment</t>
+  </si>
+  <si>
+    <t>Deleting the account created by a different manager id</t>
+  </si>
+  <si>
+    <t>Deleting the customer id created by a different manager id</t>
+  </si>
+  <si>
+    <t>Account created by a different manager id</t>
+  </si>
+  <si>
+    <t>deleted account</t>
+  </si>
+  <si>
+    <t>Unauthorized account</t>
+  </si>
+  <si>
+    <t>blank account</t>
+  </si>
+  <si>
+    <t>only spaces</t>
+  </si>
+  <si>
+    <t>special characters</t>
+  </si>
+  <si>
+    <t>characters</t>
+  </si>
+  <si>
+    <t>$%^&amp;*</t>
+  </si>
+  <si>
+    <t>Pass - You are not authorize to deposit money in this account!!</t>
+  </si>
+  <si>
+    <t>2300</t>
+  </si>
+  <si>
+    <t>2700</t>
+  </si>
+  <si>
+    <t>Pass - You Have Succesfully Logged Out!!</t>
+  </si>
+  <si>
+    <t>Exisitng account with 500 balance</t>
+  </si>
+  <si>
+    <t>Blank amount</t>
+  </si>
+  <si>
+    <t>Only spaces in amount</t>
+  </si>
+  <si>
+    <t>Characters in amount</t>
+  </si>
+  <si>
+    <t>Special characters in amount</t>
+  </si>
+  <si>
+    <t>Amount field must not be blank</t>
+  </si>
+  <si>
+    <t>Amount greater than 100000</t>
+  </si>
+  <si>
+    <t>Blank description</t>
+  </si>
+  <si>
+    <t>Description can not be blank</t>
+  </si>
+  <si>
+    <t>Only spaces in description</t>
+  </si>
+  <si>
+    <t>Numbers in description</t>
+  </si>
+  <si>
+    <t>Special characters in description</t>
+  </si>
+  <si>
+    <t>%^&amp;*(</t>
+  </si>
+  <si>
+    <t>Description exceeding 10 characters</t>
+  </si>
+  <si>
+    <t>SampleDeposit</t>
+  </si>
+  <si>
+    <t>All three fields blank</t>
+  </si>
+  <si>
+    <t>Account Number must not be blankAmount field must not be blankDescription can not be blank</t>
+  </si>
+  <si>
+    <t>Transaction details of Withdrawal for Account</t>
+  </si>
+  <si>
+    <t>You are not authorize to debit money from this account!!</t>
+  </si>
+  <si>
+    <t>HighAmount</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1348,8 +1478,28 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1455,8 +1605,58 @@
         <fgColor indexed="57"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="57"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="52"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="52">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -2223,12 +2423,132 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2309,7 +2629,10 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2319,6 +2642,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="59" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2600,10 +2945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J53"/>
+  <dimension ref="B3:J55"/>
   <sheetViews>
     <sheetView topLeftCell="H13" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2628,7 +2973,7 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="13"/>
-      <c r="H7" s="75" t="s">
+      <c r="H7" s="78" t="s">
         <v>328</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -2640,7 +2985,7 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="13"/>
-      <c r="H8" s="75"/>
+      <c r="H8" s="78"/>
       <c r="I8" s="1" t="s">
         <v>331</v>
       </c>
@@ -2650,7 +2995,7 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="25"/>
-      <c r="H9" s="75"/>
+      <c r="H9" s="78"/>
       <c r="I9" s="1" t="s">
         <v>332</v>
       </c>
@@ -2712,133 +3057,153 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="30"/>
-      <c r="H17" s="77">
+      <c r="H17" s="80">
         <v>37672</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="75">
         <v>39905</v>
       </c>
       <c r="J17" s="58"/>
     </row>
     <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="61"/>
-      <c r="H18" s="77"/>
-      <c r="I18" s="58">
+      <c r="H18" s="80"/>
+      <c r="I18" s="75">
         <v>39906</v>
       </c>
       <c r="J18" s="58"/>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="61"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="58"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="1">
+        <v>39946</v>
+      </c>
       <c r="J19" s="58"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="61"/>
-      <c r="H20" s="77"/>
-      <c r="I20" s="58"/>
+      <c r="B20" s="88"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="89">
+        <v>39947</v>
+      </c>
       <c r="J20" s="58"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="58"/>
+      <c r="B21" s="88"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="89">
+        <v>39948</v>
+      </c>
       <c r="J21" s="58"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="58"/>
+      <c r="B22" s="61"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="89">
+        <v>39949</v>
+      </c>
       <c r="J22" s="58"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="19"/>
-      <c r="H23" s="76"/>
+      <c r="B23" s="17"/>
+      <c r="H23" s="79"/>
       <c r="I23" s="58"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="20"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="21"/>
-      <c r="H25" s="76"/>
-      <c r="I25" s="1"/>
+      <c r="J23" s="58"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+    </row>
+    <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="19"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="58"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="22"/>
-      <c r="H26" s="76"/>
+      <c r="B26" s="20"/>
+      <c r="H26" s="79"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
+      <c r="B27" s="21"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="31"/>
+      <c r="B28" s="22"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="32"/>
+      <c r="B29" s="23"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="33"/>
+      <c r="B30" s="31"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="34"/>
+      <c r="B31" s="32"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="35"/>
+      <c r="B32" s="33"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="36"/>
+      <c r="B33" s="34"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="35"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="37"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="38"/>
+      <c r="B35" s="36"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="39"/>
+      <c r="B37" s="37"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="40"/>
+      <c r="B38" s="38"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="41"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="42"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="43"/>
+      <c r="B39" s="39"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="40"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="41"/>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="44"/>
+      <c r="B44" s="42"/>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="45"/>
+      <c r="B45" s="43"/>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="46"/>
+      <c r="B46" s="44"/>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="47"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="48"/>
+      <c r="B47" s="45"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="46"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="47"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="H7:H9"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="H17:H20"/>
-    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="H17:H22"/>
+    <mergeCell ref="H26:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
@@ -2846,14 +3211,495 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C2" s="91">
+        <v>39947</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="51">
+        <v>200</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C3" s="49">
+        <v>39948</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E3" s="51">
+        <v>400</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C4" s="49">
+        <v>39949</v>
+      </c>
+      <c r="D4" s="1">
+        <v>500</v>
+      </c>
+      <c r="E4" s="51"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>500</v>
+      </c>
+      <c r="E5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D6" s="1">
+        <v>500</v>
+      </c>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D7" s="1">
+        <v>500</v>
+      </c>
+      <c r="E7" s="1">
+        <v>100</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D8" s="1">
+        <v>500</v>
+      </c>
+      <c r="E8" s="1">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C9" s="1">
+        <v>39946</v>
+      </c>
+      <c r="D9" s="1">
+        <v>500</v>
+      </c>
+      <c r="E9" s="1">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="H9" s="87"/>
+      <c r="I9" s="87"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C10" s="1">
+        <v>39908</v>
+      </c>
+      <c r="D10" s="1">
+        <v>500</v>
+      </c>
+      <c r="E10" s="1">
+        <v>100</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="100" t="s">
+        <v>431</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="100" t="s">
+        <v>432</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="100" t="s">
+        <v>433</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="100" t="s">
+        <v>434</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="100" t="s">
+        <v>436</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1">
+        <v>100001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>100</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="100" t="s">
+        <v>437</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="100" t="s">
+        <v>439</v>
+      </c>
+      <c r="C17" s="49">
+        <v>39905</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2810</v>
+      </c>
+      <c r="E17" s="1">
+        <v>100</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="100" t="s">
+        <v>440</v>
+      </c>
+      <c r="C18" s="101">
+        <v>39947</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2300</v>
+      </c>
+      <c r="E18" s="1">
+        <v>150</v>
+      </c>
+      <c r="F18" s="1">
+        <v>123345</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="100" t="s">
+        <v>441</v>
+      </c>
+      <c r="C19" s="89">
+        <v>39948</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2810</v>
+      </c>
+      <c r="E19" s="1">
+        <v>200</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="100" t="s">
+        <v>443</v>
+      </c>
+      <c r="C20" s="89">
+        <v>39947</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2300</v>
+      </c>
+      <c r="E20" s="1">
+        <v>100</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="100" t="s">
+        <v>445</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2898,7 +3744,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
@@ -2909,19 +3755,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C2" s="1">
         <v>39905</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F2" s="66" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -2929,19 +3775,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C3" s="1">
         <v>39906</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E3" s="51" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="F3" s="67" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -2959,7 +3805,7 @@
         <v>385</v>
       </c>
       <c r="F4" s="68" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -2967,10 +3813,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>133</v>
@@ -2979,7 +3825,7 @@
         <v>385</v>
       </c>
       <c r="F5" s="69" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -2990,7 +3836,7 @@
         <v>373</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>133</v>
@@ -2999,7 +3845,7 @@
         <v>385</v>
       </c>
       <c r="F6" s="70" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -3010,7 +3856,7 @@
         <v>374</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>123</v>
@@ -3019,7 +3865,7 @@
         <v>385</v>
       </c>
       <c r="F7" s="71" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -3027,7 +3873,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C8" s="1">
         <v>39276</v>
@@ -3039,7 +3885,7 @@
         <v>385</v>
       </c>
       <c r="F8" s="72" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -3047,7 +3893,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C9" s="1">
         <v>34587690128</v>
@@ -3059,7 +3905,7 @@
         <v>385</v>
       </c>
       <c r="F9" s="73" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -3074,7 +3920,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -3111,7 +3957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -3159,7 +4005,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>336</v>
@@ -3167,8 +4013,8 @@
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="74" t="s">
-        <v>402</v>
+      <c r="G2" s="76" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3302,7 +4148,9 @@
       <c r="F9" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="77" t="s">
+        <v>429</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6010,8 +6858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:E26"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6380,7 +7228,9 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="53"/>
-      <c r="B27" s="52"/>
+      <c r="B27" s="74" t="s">
+        <v>417</v>
+      </c>
       <c r="C27" s="52"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -7030,10 +7880,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7337,6 +8187,11 @@
       </c>
       <c r="E21" s="51"/>
     </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="74" t="s">
+        <v>416</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
@@ -7345,101 +8200,504 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H1:U28"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="38.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="51.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="H1" s="3" t="s">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C2" s="49">
+        <v>39905</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2810</v>
+      </c>
+      <c r="E2" s="51">
+        <v>200</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="H2" s="92" t="s">
+        <v>428</v>
+      </c>
+      <c r="I2" s="92" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C3" s="49">
+        <v>39906</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E3" s="51">
+        <v>400</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="H3" s="93" t="s">
+        <v>427</v>
+      </c>
+      <c r="I3" s="93" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>500</v>
+      </c>
+      <c r="E4" s="1">
+        <v>100</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" s="94" t="s">
+        <v>385</v>
+      </c>
+      <c r="I4" s="94" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="1">
+        <v>500</v>
+      </c>
+      <c r="E5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" s="95" t="s">
+        <v>385</v>
+      </c>
+      <c r="I5" s="95" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D6" s="1">
+        <v>500</v>
+      </c>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="96" t="s">
+        <v>385</v>
+      </c>
+      <c r="I6" s="96" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D7" s="1">
+        <v>500</v>
+      </c>
+      <c r="E7" s="1">
+        <v>100</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="97" t="s">
+        <v>385</v>
+      </c>
+      <c r="I7" s="97" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C8" s="1">
+        <v>39946</v>
+      </c>
+      <c r="D8" s="1">
+        <v>500</v>
+      </c>
+      <c r="E8" s="1">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="H8" s="98" t="s">
+        <v>385</v>
+      </c>
+      <c r="I8" s="98" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C9" s="1">
+        <v>39908</v>
+      </c>
+      <c r="D9" s="1">
+        <v>500</v>
+      </c>
+      <c r="E9" s="1">
+        <v>100</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="H9" s="99" t="s">
+        <v>385</v>
+      </c>
+      <c r="I9" s="99" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="100" t="s">
+        <v>431</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="100" t="s">
+        <v>432</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="100" t="s">
+        <v>433</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="100" t="s">
+        <v>434</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="100" t="s">
+        <v>436</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1">
+        <v>100001</v>
+      </c>
+      <c r="E14" s="1">
+        <v>100</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="100" t="s">
+        <v>437</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="100" t="s">
+        <v>439</v>
+      </c>
+      <c r="C16" s="49">
+        <v>39905</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2810</v>
+      </c>
+      <c r="E16" s="1">
+        <v>100</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="100" t="s">
+        <v>440</v>
+      </c>
+      <c r="C17" s="49">
+        <v>39906</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2300</v>
+      </c>
+      <c r="E17" s="1">
+        <v>150</v>
+      </c>
+      <c r="F17" s="1">
+        <v>123345</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="8:16" x14ac:dyDescent="0.25">
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="B18" s="100" t="s">
+        <v>441</v>
+      </c>
+      <c r="C18" s="1">
         <v>39905</v>
       </c>
-      <c r="K2" s="1">
-        <v>800</v>
-      </c>
-      <c r="L2" s="1">
-        <v>250</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="23" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U23" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="24" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U24" s="65" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="26" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U26" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="27" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U27" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="28" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U28" t="s">
-        <v>414</v>
-      </c>
+      <c r="D18" s="1">
+        <v>2810</v>
+      </c>
+      <c r="E18" s="1">
+        <v>200</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="100" t="s">
+        <v>443</v>
+      </c>
+      <c r="C19" s="1">
+        <v>39906</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2300</v>
+      </c>
+      <c r="E19" s="1">
+        <v>100</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="100" t="s">
+        <v>445</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>